<commit_message>
Fixed broken page links, small adjs in ClaimResponse.
Addressed broken page links, made small profile adjustments in ClaimResponse.
</commit_message>
<xml_diff>
--- a/output/carin-rtpbc-ClaimResponse.xlsx
+++ b/output/carin-rtpbc-ClaimResponse.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8284" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8284" uniqueCount="854">
   <si>
     <t>Path</t>
   </si>
@@ -1271,7 +1271,7 @@
     <t>RTPBC Patient Pay Categories</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/carin/ValueSet/rtpbc-patient-pay-category</t>
+    <t>http://hl7.org/fhir/us/carin/ValueSet/rtpbc-patient-pay-type</t>
   </si>
   <si>
     <t>ClaimResponse.item.adjudication.reason</t>
@@ -1583,6 +1583,9 @@
     <t>CARIN RTPBC prescribable product codes (NDC and RxNorm)</t>
   </si>
   <si>
+    <t>http://hl7.org/fhir/us/carin/ValueSet/carin-rtpbc-prescribable-product-code</t>
+  </si>
+  <si>
     <t>ClaimResponse.addItem.productOrService.id</t>
   </si>
   <si>
@@ -1806,6 +1809,9 @@
   </si>
   <si>
     <t>Billing quantity unity of measure</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/carin/ValueSet/rtpbc-billing-units</t>
   </si>
   <si>
     <t>Quantity.unit</t>
@@ -2806,7 +2812,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="121.30859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="59.26171875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="69.37890625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
@@ -15712,7 +15718,7 @@
         <v>506</v>
       </c>
       <c r="Y119" t="s" s="2">
-        <v>42</v>
+        <v>507</v>
       </c>
       <c r="Z119" t="s" s="2">
         <v>42</v>
@@ -15756,7 +15762,7 @@
     </row>
     <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" t="s" s="2">
@@ -15862,7 +15868,7 @@
     </row>
     <row r="121" hidden="true">
       <c r="A121" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B121" s="2"/>
       <c r="C121" t="s" s="2">
@@ -15970,7 +15976,7 @@
     </row>
     <row r="122">
       <c r="A122" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" t="s" s="2">
@@ -16080,7 +16086,7 @@
     </row>
     <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" t="s" s="2">
@@ -16186,7 +16192,7 @@
     </row>
     <row r="124" hidden="true">
       <c r="A124" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" t="s" s="2">
@@ -16294,7 +16300,7 @@
     </row>
     <row r="125">
       <c r="A125" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" t="s" s="2">
@@ -16404,7 +16410,7 @@
     </row>
     <row r="126" hidden="true">
       <c r="A126" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" t="s" s="2">
@@ -16512,7 +16518,7 @@
     </row>
     <row r="127">
       <c r="A127" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" t="s" s="2">
@@ -16620,14 +16626,14 @@
     </row>
     <row r="128">
       <c r="A128" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D128" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E128" t="s" s="2">
         <v>50</v>
@@ -16648,10 +16654,10 @@
         <v>52</v>
       </c>
       <c r="K128" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="L128" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="M128" s="2"/>
       <c r="N128" t="s" s="2">
@@ -16730,7 +16736,7 @@
     </row>
     <row r="129" hidden="true">
       <c r="A129" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" t="s" s="2">
@@ -16840,7 +16846,7 @@
     </row>
     <row r="130" hidden="true">
       <c r="A130" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" t="s" s="2">
@@ -16950,7 +16956,7 @@
     </row>
     <row r="131" hidden="true">
       <c r="A131" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B131" s="2"/>
       <c r="C131" t="s" s="2">
@@ -16976,16 +16982,16 @@
         <v>135</v>
       </c>
       <c r="K131" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="L131" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="M131" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="N131" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="O131" t="s" s="2">
         <v>42</v>
@@ -17013,10 +17019,10 @@
         <v>247</v>
       </c>
       <c r="X131" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="Y131" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="Z131" t="s" s="2">
         <v>42</v>
@@ -17034,7 +17040,7 @@
         <v>42</v>
       </c>
       <c r="AE131" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="AF131" t="s" s="2">
         <v>40</v>
@@ -17055,12 +17061,12 @@
         <v>42</v>
       </c>
       <c r="AL131" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="132" hidden="true">
       <c r="A132" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B132" s="2"/>
       <c r="C132" t="s" s="2">
@@ -17086,16 +17092,16 @@
         <v>135</v>
       </c>
       <c r="K132" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="L132" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="M132" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="N132" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="O132" t="s" s="2">
         <v>42</v>
@@ -17123,10 +17129,10 @@
         <v>247</v>
       </c>
       <c r="X132" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="Y132" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="Z132" t="s" s="2">
         <v>42</v>
@@ -17144,7 +17150,7 @@
         <v>42</v>
       </c>
       <c r="AE132" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="AF132" t="s" s="2">
         <v>40</v>
@@ -17165,12 +17171,12 @@
         <v>42</v>
       </c>
       <c r="AL132" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="133" hidden="true">
       <c r="A133" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B133" s="2"/>
       <c r="C133" t="s" s="2">
@@ -17193,17 +17199,17 @@
         <v>42</v>
       </c>
       <c r="J133" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="K133" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="L133" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="M133" s="2"/>
       <c r="N133" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="O133" t="s" s="2">
         <v>42</v>
@@ -17252,7 +17258,7 @@
         <v>42</v>
       </c>
       <c r="AE133" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="AF133" t="s" s="2">
         <v>40</v>
@@ -17270,15 +17276,15 @@
         <v>42</v>
       </c>
       <c r="AK133" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="AL133" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="134" hidden="true">
       <c r="A134" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" t="s" s="2">
@@ -17301,17 +17307,17 @@
         <v>42</v>
       </c>
       <c r="J134" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="K134" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="L134" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M134" s="2"/>
       <c r="N134" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="O134" t="s" s="2">
         <v>42</v>
@@ -17339,10 +17345,10 @@
         <v>247</v>
       </c>
       <c r="X134" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="Y134" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="Z134" t="s" s="2">
         <v>42</v>
@@ -17360,7 +17366,7 @@
         <v>42</v>
       </c>
       <c r="AE134" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="AF134" t="s" s="2">
         <v>40</v>
@@ -17378,22 +17384,22 @@
         <v>42</v>
       </c>
       <c r="AK134" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="AL134" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D135" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E135" t="s" s="2">
         <v>50</v>
@@ -17411,17 +17417,17 @@
         <v>42</v>
       </c>
       <c r="J135" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="K135" t="s" s="2">
         <v>554</v>
       </c>
-      <c r="K135" t="s" s="2">
-        <v>553</v>
-      </c>
       <c r="L135" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="M135" s="2"/>
       <c r="N135" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="O135" t="s" s="2">
         <v>42</v>
@@ -17470,7 +17476,7 @@
         <v>42</v>
       </c>
       <c r="AE135" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="AF135" t="s" s="2">
         <v>40</v>
@@ -17491,12 +17497,12 @@
         <v>42</v>
       </c>
       <c r="AL135" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="136" hidden="true">
       <c r="A136" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" t="s" s="2">
@@ -17602,7 +17608,7 @@
     </row>
     <row r="137" hidden="true">
       <c r="A137" t="s" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B137" s="2"/>
       <c r="C137" t="s" s="2">
@@ -17710,14 +17716,14 @@
     </row>
     <row r="138">
       <c r="A138" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B138" s="2"/>
       <c r="C138" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D138" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E138" t="s" s="2">
         <v>50</v>
@@ -17738,16 +17744,16 @@
         <v>422</v>
       </c>
       <c r="K138" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="L138" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="M138" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="N138" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="O138" t="s" s="2">
         <v>42</v>
@@ -17796,7 +17802,7 @@
         <v>42</v>
       </c>
       <c r="AE138" t="s" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="AF138" t="s" s="2">
         <v>40</v>
@@ -17817,12 +17823,12 @@
         <v>42</v>
       </c>
       <c r="AL138" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="139" hidden="true">
       <c r="A139" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B139" s="2"/>
       <c r="C139" t="s" s="2">
@@ -17848,20 +17854,20 @@
         <v>69</v>
       </c>
       <c r="K139" t="s" s="2">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="L139" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="M139" s="2"/>
       <c r="N139" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="O139" t="s" s="2">
         <v>42</v>
       </c>
       <c r="P139" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="Q139" t="s" s="2">
         <v>42</v>
@@ -17885,10 +17891,10 @@
         <v>129</v>
       </c>
       <c r="X139" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="Y139" t="s" s="2">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="Z139" t="s" s="2">
         <v>42</v>
@@ -17906,7 +17912,7 @@
         <v>42</v>
       </c>
       <c r="AE139" t="s" s="2">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="AF139" t="s" s="2">
         <v>40</v>
@@ -17927,19 +17933,19 @@
         <v>42</v>
       </c>
       <c r="AL139" t="s" s="2">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D140" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="E140" t="s" s="2">
         <v>50</v>
@@ -17960,14 +17966,14 @@
         <v>52</v>
       </c>
       <c r="K140" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="L140" t="s" s="2">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="M140" s="2"/>
       <c r="N140" t="s" s="2">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="O140" t="s" s="2">
         <v>42</v>
@@ -17995,10 +18001,10 @@
         <v>129</v>
       </c>
       <c r="X140" t="s" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="Y140" t="s" s="2">
-        <v>42</v>
+        <v>582</v>
       </c>
       <c r="Z140" t="s" s="2">
         <v>42</v>
@@ -18016,7 +18022,7 @@
         <v>42</v>
       </c>
       <c r="AE140" t="s" s="2">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="AF140" t="s" s="2">
         <v>40</v>
@@ -18037,12 +18043,12 @@
         <v>42</v>
       </c>
       <c r="AL140" t="s" s="2">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="141" hidden="true">
       <c r="A141" t="s" s="2">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" t="s" s="2">
@@ -18068,14 +18074,14 @@
         <v>63</v>
       </c>
       <c r="K141" t="s" s="2">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="L141" t="s" s="2">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="M141" s="2"/>
       <c r="N141" t="s" s="2">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="O141" t="s" s="2">
         <v>42</v>
@@ -18124,7 +18130,7 @@
         <v>42</v>
       </c>
       <c r="AE141" t="s" s="2">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="AF141" t="s" s="2">
         <v>40</v>
@@ -18133,7 +18139,7 @@
         <v>50</v>
       </c>
       <c r="AH141" t="s" s="2">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="AI141" t="s" s="2">
         <v>61</v>
@@ -18145,12 +18151,12 @@
         <v>42</v>
       </c>
       <c r="AL141" t="s" s="2">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="142" hidden="true">
       <c r="A142" t="s" s="2">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" t="s" s="2">
@@ -18176,16 +18182,16 @@
         <v>69</v>
       </c>
       <c r="K142" t="s" s="2">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="L142" t="s" s="2">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="M142" t="s" s="2">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="N142" t="s" s="2">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="O142" t="s" s="2">
         <v>42</v>
@@ -18234,7 +18240,7 @@
         <v>42</v>
       </c>
       <c r="AE142" t="s" s="2">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="AF142" t="s" s="2">
         <v>40</v>
@@ -18255,12 +18261,12 @@
         <v>42</v>
       </c>
       <c r="AL142" t="s" s="2">
-        <v>596</v>
+        <v>598</v>
       </c>
     </row>
     <row r="143" hidden="true">
       <c r="A143" t="s" s="2">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" t="s" s="2">
@@ -18286,14 +18292,14 @@
         <v>414</v>
       </c>
       <c r="K143" t="s" s="2">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="L143" t="s" s="2">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="M143" s="2"/>
       <c r="N143" t="s" s="2">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="O143" t="s" s="2">
         <v>42</v>
@@ -18342,7 +18348,7 @@
         <v>42</v>
       </c>
       <c r="AE143" t="s" s="2">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="AF143" t="s" s="2">
         <v>40</v>
@@ -18368,7 +18374,7 @@
     </row>
     <row r="144" hidden="true">
       <c r="A144" t="s" s="2">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" t="s" s="2">
@@ -18394,16 +18400,16 @@
         <v>422</v>
       </c>
       <c r="K144" t="s" s="2">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="L144" t="s" s="2">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="M144" t="s" s="2">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="N144" t="s" s="2">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="O144" t="s" s="2">
         <v>42</v>
@@ -18452,7 +18458,7 @@
         <v>42</v>
       </c>
       <c r="AE144" t="s" s="2">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="AF144" t="s" s="2">
         <v>40</v>
@@ -18478,7 +18484,7 @@
     </row>
     <row r="145" hidden="true">
       <c r="A145" t="s" s="2">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" t="s" s="2">
@@ -18504,16 +18510,16 @@
         <v>414</v>
       </c>
       <c r="K145" t="s" s="2">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="L145" t="s" s="2">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="M145" t="s" s="2">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="N145" t="s" s="2">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="O145" t="s" s="2">
         <v>42</v>
@@ -18562,7 +18568,7 @@
         <v>42</v>
       </c>
       <c r="AE145" t="s" s="2">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="AF145" t="s" s="2">
         <v>40</v>
@@ -18583,12 +18589,12 @@
         <v>42</v>
       </c>
       <c r="AL145" t="s" s="2">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="146" hidden="true">
       <c r="A146" t="s" s="2">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" t="s" s="2">
@@ -18614,16 +18620,16 @@
         <v>135</v>
       </c>
       <c r="K146" t="s" s="2">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="L146" t="s" s="2">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="M146" t="s" s="2">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="N146" t="s" s="2">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="O146" t="s" s="2">
         <v>42</v>
@@ -18651,10 +18657,10 @@
         <v>247</v>
       </c>
       <c r="X146" t="s" s="2">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="Y146" t="s" s="2">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="Z146" t="s" s="2">
         <v>42</v>
@@ -18672,7 +18678,7 @@
         <v>42</v>
       </c>
       <c r="AE146" t="s" s="2">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="AF146" t="s" s="2">
         <v>40</v>
@@ -18698,7 +18704,7 @@
     </row>
     <row r="147" hidden="true">
       <c r="A147" t="s" s="2">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" t="s" s="2">
@@ -18724,14 +18730,14 @@
         <v>135</v>
       </c>
       <c r="K147" t="s" s="2">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="L147" t="s" s="2">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="M147" s="2"/>
       <c r="N147" t="s" s="2">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="O147" t="s" s="2">
         <v>42</v>
@@ -18759,10 +18765,10 @@
         <v>247</v>
       </c>
       <c r="X147" t="s" s="2">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="Y147" t="s" s="2">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="Z147" t="s" s="2">
         <v>42</v>
@@ -18780,7 +18786,7 @@
         <v>42</v>
       </c>
       <c r="AE147" t="s" s="2">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="AF147" t="s" s="2">
         <v>40</v>
@@ -18806,7 +18812,7 @@
     </row>
     <row r="148">
       <c r="A148" t="s" s="2">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" t="s" s="2">
@@ -18890,7 +18896,7 @@
         <v>42</v>
       </c>
       <c r="AE148" t="s" s="2">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="AF148" t="s" s="2">
         <v>40</v>
@@ -18916,14 +18922,14 @@
     </row>
     <row r="149">
       <c r="A149" t="s" s="2">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="B149" s="2"/>
       <c r="C149" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D149" t="s" s="2">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="E149" t="s" s="2">
         <v>50</v>
@@ -18944,10 +18950,10 @@
         <v>371</v>
       </c>
       <c r="K149" t="s" s="2">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="L149" t="s" s="2">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="M149" s="2"/>
       <c r="N149" s="2"/>
@@ -18998,7 +19004,7 @@
         <v>42</v>
       </c>
       <c r="AE149" t="s" s="2">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="AF149" t="s" s="2">
         <v>50</v>
@@ -19024,7 +19030,7 @@
     </row>
     <row r="150" hidden="true">
       <c r="A150" t="s" s="2">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" t="s" s="2">
@@ -19130,7 +19136,7 @@
     </row>
     <row r="151" hidden="true">
       <c r="A151" t="s" s="2">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="B151" s="2"/>
       <c r="C151" t="s" s="2">
@@ -19238,7 +19244,7 @@
     </row>
     <row r="152" hidden="true">
       <c r="A152" t="s" s="2">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" t="s" s="2">
@@ -19348,7 +19354,7 @@
     </row>
     <row r="153">
       <c r="A153" t="s" s="2">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="B153" s="2"/>
       <c r="C153" t="s" s="2">
@@ -19460,7 +19466,7 @@
     </row>
     <row r="154" hidden="true">
       <c r="A154" t="s" s="2">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="B154" s="2"/>
       <c r="C154" t="s" s="2">
@@ -19570,7 +19576,7 @@
     </row>
     <row r="155">
       <c r="A155" t="s" s="2">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="B155" s="2"/>
       <c r="C155" t="s" s="2">
@@ -19682,7 +19688,7 @@
     </row>
     <row r="156" hidden="true">
       <c r="A156" t="s" s="2">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" t="s" s="2">
@@ -19788,7 +19794,7 @@
     </row>
     <row r="157" hidden="true">
       <c r="A157" t="s" s="2">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="B157" s="2"/>
       <c r="C157" t="s" s="2">
@@ -19896,7 +19902,7 @@
     </row>
     <row r="158">
       <c r="A158" t="s" s="2">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" t="s" s="2">
@@ -20008,7 +20014,7 @@
     </row>
     <row r="159">
       <c r="A159" t="s" s="2">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" t="s" s="2">
@@ -20118,7 +20124,7 @@
     </row>
     <row r="160" hidden="true">
       <c r="A160" t="s" s="2">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" t="s" s="2">
@@ -20228,7 +20234,7 @@
     </row>
     <row r="161" hidden="true">
       <c r="A161" t="s" s="2">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="B161" s="2"/>
       <c r="C161" t="s" s="2">
@@ -20254,10 +20260,10 @@
         <v>371</v>
       </c>
       <c r="K161" t="s" s="2">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="L161" t="s" s="2">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="M161" s="2"/>
       <c r="N161" s="2"/>
@@ -20308,7 +20314,7 @@
         <v>42</v>
       </c>
       <c r="AE161" t="s" s="2">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="AF161" t="s" s="2">
         <v>40</v>
@@ -20334,7 +20340,7 @@
     </row>
     <row r="162" hidden="true">
       <c r="A162" t="s" s="2">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" t="s" s="2">
@@ -20440,7 +20446,7 @@
     </row>
     <row r="163" hidden="true">
       <c r="A163" t="s" s="2">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" t="s" s="2">
@@ -20548,7 +20554,7 @@
     </row>
     <row r="164" hidden="true">
       <c r="A164" t="s" s="2">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="B164" s="2"/>
       <c r="C164" t="s" s="2">
@@ -20658,7 +20664,7 @@
     </row>
     <row r="165" hidden="true">
       <c r="A165" t="s" s="2">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" t="s" s="2">
@@ -20684,10 +20690,10 @@
         <v>135</v>
       </c>
       <c r="K165" t="s" s="2">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="L165" t="s" s="2">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="M165" t="s" s="2">
         <v>504</v>
@@ -20721,10 +20727,10 @@
         <v>247</v>
       </c>
       <c r="X165" t="s" s="2">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="Y165" t="s" s="2">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="Z165" t="s" s="2">
         <v>42</v>
@@ -20742,7 +20748,7 @@
         <v>42</v>
       </c>
       <c r="AE165" t="s" s="2">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="AF165" t="s" s="2">
         <v>50</v>
@@ -20768,7 +20774,7 @@
     </row>
     <row r="166" hidden="true">
       <c r="A166" t="s" s="2">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="B166" s="2"/>
       <c r="C166" t="s" s="2">
@@ -20794,16 +20800,16 @@
         <v>135</v>
       </c>
       <c r="K166" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="L166" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="M166" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="N166" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="O166" t="s" s="2">
         <v>42</v>
@@ -20831,10 +20837,10 @@
         <v>247</v>
       </c>
       <c r="X166" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="Y166" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="Z166" t="s" s="2">
         <v>42</v>
@@ -20852,7 +20858,7 @@
         <v>42</v>
       </c>
       <c r="AE166" t="s" s="2">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="AF166" t="s" s="2">
         <v>40</v>
@@ -20873,12 +20879,12 @@
         <v>42</v>
       </c>
       <c r="AL166" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="167" hidden="true">
       <c r="A167" t="s" s="2">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" t="s" s="2">
@@ -20901,17 +20907,17 @@
         <v>42</v>
       </c>
       <c r="J167" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="K167" t="s" s="2">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="L167" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="M167" s="2"/>
       <c r="N167" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="O167" t="s" s="2">
         <v>42</v>
@@ -20960,7 +20966,7 @@
         <v>42</v>
       </c>
       <c r="AE167" t="s" s="2">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="AF167" t="s" s="2">
         <v>40</v>
@@ -20981,12 +20987,12 @@
         <v>42</v>
       </c>
       <c r="AL167" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="168" hidden="true">
       <c r="A168" t="s" s="2">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="B168" s="2"/>
       <c r="C168" t="s" s="2">
@@ -21012,14 +21018,14 @@
         <v>414</v>
       </c>
       <c r="K168" t="s" s="2">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="L168" t="s" s="2">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="M168" s="2"/>
       <c r="N168" t="s" s="2">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="O168" t="s" s="2">
         <v>42</v>
@@ -21068,7 +21074,7 @@
         <v>42</v>
       </c>
       <c r="AE168" t="s" s="2">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="AF168" t="s" s="2">
         <v>40</v>
@@ -21094,7 +21100,7 @@
     </row>
     <row r="169" hidden="true">
       <c r="A169" t="s" s="2">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" t="s" s="2">
@@ -21120,16 +21126,16 @@
         <v>422</v>
       </c>
       <c r="K169" t="s" s="2">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="L169" t="s" s="2">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="M169" t="s" s="2">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="N169" t="s" s="2">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="O169" t="s" s="2">
         <v>42</v>
@@ -21178,7 +21184,7 @@
         <v>42</v>
       </c>
       <c r="AE169" t="s" s="2">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="AF169" t="s" s="2">
         <v>40</v>
@@ -21204,7 +21210,7 @@
     </row>
     <row r="170" hidden="true">
       <c r="A170" t="s" s="2">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="B170" s="2"/>
       <c r="C170" t="s" s="2">
@@ -21230,16 +21236,16 @@
         <v>414</v>
       </c>
       <c r="K170" t="s" s="2">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="L170" t="s" s="2">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="M170" t="s" s="2">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="N170" t="s" s="2">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="O170" t="s" s="2">
         <v>42</v>
@@ -21288,7 +21294,7 @@
         <v>42</v>
       </c>
       <c r="AE170" t="s" s="2">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="AF170" t="s" s="2">
         <v>40</v>
@@ -21309,12 +21315,12 @@
         <v>42</v>
       </c>
       <c r="AL170" t="s" s="2">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="171" hidden="true">
       <c r="A171" t="s" s="2">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="B171" s="2"/>
       <c r="C171" t="s" s="2">
@@ -21396,7 +21402,7 @@
         <v>42</v>
       </c>
       <c r="AE171" t="s" s="2">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="AF171" t="s" s="2">
         <v>40</v>
@@ -21422,7 +21428,7 @@
     </row>
     <row r="172" hidden="true">
       <c r="A172" t="s" s="2">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="B172" s="2"/>
       <c r="C172" t="s" s="2">
@@ -21448,7 +21454,7 @@
         <v>42</v>
       </c>
       <c r="K172" t="s" s="2">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="L172" t="s" s="2">
         <v>454</v>
@@ -21502,7 +21508,7 @@
         <v>42</v>
       </c>
       <c r="AE172" t="s" s="2">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="AF172" t="s" s="2">
         <v>50</v>
@@ -21528,7 +21534,7 @@
     </row>
     <row r="173" hidden="true">
       <c r="A173" t="s" s="2">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="B173" s="2"/>
       <c r="C173" t="s" s="2">
@@ -21557,7 +21563,7 @@
         <v>470</v>
       </c>
       <c r="L173" t="s" s="2">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="M173" s="2"/>
       <c r="N173" s="2"/>
@@ -21608,7 +21614,7 @@
         <v>42</v>
       </c>
       <c r="AE173" t="s" s="2">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="AF173" t="s" s="2">
         <v>40</v>
@@ -21634,7 +21640,7 @@
     </row>
     <row r="174" hidden="true">
       <c r="A174" t="s" s="2">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="B174" s="2"/>
       <c r="C174" t="s" s="2">
@@ -21740,7 +21746,7 @@
     </row>
     <row r="175" hidden="true">
       <c r="A175" t="s" s="2">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="B175" s="2"/>
       <c r="C175" t="s" s="2">
@@ -21848,7 +21854,7 @@
     </row>
     <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" t="s" s="2">
@@ -21958,7 +21964,7 @@
     </row>
     <row r="177" hidden="true">
       <c r="A177" t="s" s="2">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" t="s" s="2">
@@ -21984,10 +21990,10 @@
         <v>135</v>
       </c>
       <c r="K177" t="s" s="2">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="L177" t="s" s="2">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="M177" t="s" s="2">
         <v>504</v>
@@ -22021,10 +22027,10 @@
         <v>247</v>
       </c>
       <c r="X177" t="s" s="2">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="Y177" t="s" s="2">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="Z177" t="s" s="2">
         <v>42</v>
@@ -22042,7 +22048,7 @@
         <v>42</v>
       </c>
       <c r="AE177" t="s" s="2">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="AF177" t="s" s="2">
         <v>50</v>
@@ -22068,7 +22074,7 @@
     </row>
     <row r="178" hidden="true">
       <c r="A178" t="s" s="2">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="B178" s="2"/>
       <c r="C178" t="s" s="2">
@@ -22094,16 +22100,16 @@
         <v>135</v>
       </c>
       <c r="K178" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="L178" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="M178" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="N178" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="O178" t="s" s="2">
         <v>42</v>
@@ -22131,10 +22137,10 @@
         <v>247</v>
       </c>
       <c r="X178" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="Y178" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="Z178" t="s" s="2">
         <v>42</v>
@@ -22152,7 +22158,7 @@
         <v>42</v>
       </c>
       <c r="AE178" t="s" s="2">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="AF178" t="s" s="2">
         <v>40</v>
@@ -22173,12 +22179,12 @@
         <v>42</v>
       </c>
       <c r="AL178" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="179" hidden="true">
       <c r="A179" t="s" s="2">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="B179" s="2"/>
       <c r="C179" t="s" s="2">
@@ -22201,17 +22207,17 @@
         <v>42</v>
       </c>
       <c r="J179" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="K179" t="s" s="2">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="L179" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="M179" s="2"/>
       <c r="N179" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="O179" t="s" s="2">
         <v>42</v>
@@ -22260,7 +22266,7 @@
         <v>42</v>
       </c>
       <c r="AE179" t="s" s="2">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="AF179" t="s" s="2">
         <v>40</v>
@@ -22281,12 +22287,12 @@
         <v>42</v>
       </c>
       <c r="AL179" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="180" hidden="true">
       <c r="A180" t="s" s="2">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="B180" s="2"/>
       <c r="C180" t="s" s="2">
@@ -22312,14 +22318,14 @@
         <v>414</v>
       </c>
       <c r="K180" t="s" s="2">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="L180" t="s" s="2">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="M180" s="2"/>
       <c r="N180" t="s" s="2">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="O180" t="s" s="2">
         <v>42</v>
@@ -22368,7 +22374,7 @@
         <v>42</v>
       </c>
       <c r="AE180" t="s" s="2">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="AF180" t="s" s="2">
         <v>40</v>
@@ -22394,7 +22400,7 @@
     </row>
     <row r="181" hidden="true">
       <c r="A181" t="s" s="2">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="B181" s="2"/>
       <c r="C181" t="s" s="2">
@@ -22420,16 +22426,16 @@
         <v>422</v>
       </c>
       <c r="K181" t="s" s="2">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="L181" t="s" s="2">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="M181" t="s" s="2">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="N181" t="s" s="2">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="O181" t="s" s="2">
         <v>42</v>
@@ -22478,7 +22484,7 @@
         <v>42</v>
       </c>
       <c r="AE181" t="s" s="2">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="AF181" t="s" s="2">
         <v>40</v>
@@ -22504,7 +22510,7 @@
     </row>
     <row r="182" hidden="true">
       <c r="A182" t="s" s="2">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="B182" s="2"/>
       <c r="C182" t="s" s="2">
@@ -22530,16 +22536,16 @@
         <v>414</v>
       </c>
       <c r="K182" t="s" s="2">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="L182" t="s" s="2">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="M182" t="s" s="2">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="N182" t="s" s="2">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="O182" t="s" s="2">
         <v>42</v>
@@ -22588,7 +22594,7 @@
         <v>42</v>
       </c>
       <c r="AE182" t="s" s="2">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="AF182" t="s" s="2">
         <v>40</v>
@@ -22609,12 +22615,12 @@
         <v>42</v>
       </c>
       <c r="AL182" t="s" s="2">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="183" hidden="true">
       <c r="A183" t="s" s="2">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="B183" s="2"/>
       <c r="C183" t="s" s="2">
@@ -22696,7 +22702,7 @@
         <v>42</v>
       </c>
       <c r="AE183" t="s" s="2">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="AF183" t="s" s="2">
         <v>40</v>
@@ -22722,7 +22728,7 @@
     </row>
     <row r="184" hidden="true">
       <c r="A184" t="s" s="2">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="B184" s="2"/>
       <c r="C184" t="s" s="2">
@@ -22748,7 +22754,7 @@
         <v>42</v>
       </c>
       <c r="K184" t="s" s="2">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="L184" t="s" s="2">
         <v>454</v>
@@ -22802,7 +22808,7 @@
         <v>42</v>
       </c>
       <c r="AE184" t="s" s="2">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="AF184" t="s" s="2">
         <v>50</v>
@@ -22828,7 +22834,7 @@
     </row>
     <row r="185" hidden="true">
       <c r="A185" t="s" s="2">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="B185" s="2"/>
       <c r="C185" t="s" s="2">
@@ -22854,14 +22860,14 @@
         <v>42</v>
       </c>
       <c r="K185" t="s" s="2">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="L185" t="s" s="2">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="M185" s="2"/>
       <c r="N185" t="s" s="2">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="O185" t="s" s="2">
         <v>42</v>
@@ -22910,7 +22916,7 @@
         <v>42</v>
       </c>
       <c r="AE185" t="s" s="2">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="AF185" t="s" s="2">
         <v>40</v>
@@ -22936,7 +22942,7 @@
     </row>
     <row r="186" hidden="true">
       <c r="A186" t="s" s="2">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="B186" s="2"/>
       <c r="C186" t="s" s="2">
@@ -22962,16 +22968,16 @@
         <v>371</v>
       </c>
       <c r="K186" t="s" s="2">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="L186" t="s" s="2">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="M186" t="s" s="2">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="N186" t="s" s="2">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="O186" t="s" s="2">
         <v>42</v>
@@ -23020,7 +23026,7 @@
         <v>42</v>
       </c>
       <c r="AE186" t="s" s="2">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="AF186" t="s" s="2">
         <v>40</v>
@@ -23046,7 +23052,7 @@
     </row>
     <row r="187" hidden="true">
       <c r="A187" t="s" s="2">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="B187" s="2"/>
       <c r="C187" t="s" s="2">
@@ -23152,7 +23158,7 @@
     </row>
     <row r="188" hidden="true">
       <c r="A188" t="s" s="2">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="B188" s="2"/>
       <c r="C188" t="s" s="2">
@@ -23260,7 +23266,7 @@
     </row>
     <row r="189" hidden="true">
       <c r="A189" t="s" s="2">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="B189" s="2"/>
       <c r="C189" t="s" s="2">
@@ -23370,7 +23376,7 @@
     </row>
     <row r="190" hidden="true">
       <c r="A190" t="s" s="2">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="B190" s="2"/>
       <c r="C190" t="s" s="2">
@@ -23396,16 +23402,16 @@
         <v>135</v>
       </c>
       <c r="K190" t="s" s="2">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="L190" t="s" s="2">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="M190" t="s" s="2">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="N190" t="s" s="2">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="O190" t="s" s="2">
         <v>42</v>
@@ -23433,10 +23439,10 @@
         <v>247</v>
       </c>
       <c r="X190" t="s" s="2">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="Y190" t="s" s="2">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="Z190" t="s" s="2">
         <v>42</v>
@@ -23454,7 +23460,7 @@
         <v>42</v>
       </c>
       <c r="AE190" t="s" s="2">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="AF190" t="s" s="2">
         <v>50</v>
@@ -23480,7 +23486,7 @@
     </row>
     <row r="191" hidden="true">
       <c r="A191" t="s" s="2">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B191" s="2"/>
       <c r="C191" t="s" s="2">
@@ -23506,14 +23512,14 @@
         <v>414</v>
       </c>
       <c r="K191" t="s" s="2">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="L191" t="s" s="2">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="M191" s="2"/>
       <c r="N191" t="s" s="2">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="O191" t="s" s="2">
         <v>42</v>
@@ -23562,7 +23568,7 @@
         <v>42</v>
       </c>
       <c r="AE191" t="s" s="2">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="AF191" t="s" s="2">
         <v>50</v>
@@ -23588,7 +23594,7 @@
     </row>
     <row r="192" hidden="true">
       <c r="A192" t="s" s="2">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="B192" s="2"/>
       <c r="C192" t="s" s="2">
@@ -23614,14 +23620,14 @@
         <v>371</v>
       </c>
       <c r="K192" t="s" s="2">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="L192" t="s" s="2">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="M192" s="2"/>
       <c r="N192" t="s" s="2">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="O192" t="s" s="2">
         <v>42</v>
@@ -23670,7 +23676,7 @@
         <v>42</v>
       </c>
       <c r="AE192" t="s" s="2">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="AF192" t="s" s="2">
         <v>40</v>
@@ -23696,7 +23702,7 @@
     </row>
     <row r="193" hidden="true">
       <c r="A193" t="s" s="2">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="B193" s="2"/>
       <c r="C193" t="s" s="2">
@@ -23802,7 +23808,7 @@
     </row>
     <row r="194" hidden="true">
       <c r="A194" t="s" s="2">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B194" s="2"/>
       <c r="C194" t="s" s="2">
@@ -23910,7 +23916,7 @@
     </row>
     <row r="195" hidden="true">
       <c r="A195" t="s" s="2">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="B195" s="2"/>
       <c r="C195" t="s" s="2">
@@ -24020,7 +24026,7 @@
     </row>
     <row r="196" hidden="true">
       <c r="A196" t="s" s="2">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B196" s="2"/>
       <c r="C196" t="s" s="2">
@@ -24046,14 +24052,14 @@
         <v>135</v>
       </c>
       <c r="K196" t="s" s="2">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="L196" t="s" s="2">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="M196" s="2"/>
       <c r="N196" t="s" s="2">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="O196" t="s" s="2">
         <v>42</v>
@@ -24081,10 +24087,10 @@
         <v>247</v>
       </c>
       <c r="X196" t="s" s="2">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="Y196" t="s" s="2">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="Z196" t="s" s="2">
         <v>42</v>
@@ -24102,7 +24108,7 @@
         <v>42</v>
       </c>
       <c r="AE196" t="s" s="2">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="AF196" t="s" s="2">
         <v>50</v>
@@ -24128,7 +24134,7 @@
     </row>
     <row r="197" hidden="true">
       <c r="A197" t="s" s="2">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="B197" s="2"/>
       <c r="C197" t="s" s="2">
@@ -24154,16 +24160,16 @@
         <v>414</v>
       </c>
       <c r="K197" t="s" s="2">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="L197" t="s" s="2">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="M197" t="s" s="2">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="N197" t="s" s="2">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="O197" t="s" s="2">
         <v>42</v>
@@ -24212,7 +24218,7 @@
         <v>42</v>
       </c>
       <c r="AE197" t="s" s="2">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="AF197" t="s" s="2">
         <v>40</v>
@@ -24238,7 +24244,7 @@
     </row>
     <row r="198" hidden="true">
       <c r="A198" t="s" s="2">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="B198" s="2"/>
       <c r="C198" t="s" s="2">
@@ -24264,14 +24270,14 @@
         <v>135</v>
       </c>
       <c r="K198" t="s" s="2">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="L198" t="s" s="2">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="M198" s="2"/>
       <c r="N198" t="s" s="2">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="O198" t="s" s="2">
         <v>42</v>
@@ -24299,10 +24305,10 @@
         <v>247</v>
       </c>
       <c r="X198" t="s" s="2">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="Y198" t="s" s="2">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="Z198" t="s" s="2">
         <v>42</v>
@@ -24320,7 +24326,7 @@
         <v>42</v>
       </c>
       <c r="AE198" t="s" s="2">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="AF198" t="s" s="2">
         <v>40</v>
@@ -24346,7 +24352,7 @@
     </row>
     <row r="199" hidden="true">
       <c r="A199" t="s" s="2">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B199" s="2"/>
       <c r="C199" t="s" s="2">
@@ -24369,17 +24375,17 @@
         <v>42</v>
       </c>
       <c r="J199" t="s" s="2">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="K199" t="s" s="2">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="L199" t="s" s="2">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="M199" s="2"/>
       <c r="N199" t="s" s="2">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="O199" t="s" s="2">
         <v>42</v>
@@ -24428,7 +24434,7 @@
         <v>42</v>
       </c>
       <c r="AE199" t="s" s="2">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="AF199" t="s" s="2">
         <v>40</v>
@@ -24454,7 +24460,7 @@
     </row>
     <row r="200" hidden="true">
       <c r="A200" t="s" s="2">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="B200" s="2"/>
       <c r="C200" t="s" s="2">
@@ -24480,14 +24486,14 @@
         <v>414</v>
       </c>
       <c r="K200" t="s" s="2">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="L200" t="s" s="2">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="M200" s="2"/>
       <c r="N200" t="s" s="2">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="O200" t="s" s="2">
         <v>42</v>
@@ -24536,7 +24542,7 @@
         <v>42</v>
       </c>
       <c r="AE200" t="s" s="2">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="AF200" t="s" s="2">
         <v>50</v>
@@ -24562,7 +24568,7 @@
     </row>
     <row r="201" hidden="true">
       <c r="A201" t="s" s="2">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="B201" s="2"/>
       <c r="C201" t="s" s="2">
@@ -24588,16 +24594,16 @@
         <v>108</v>
       </c>
       <c r="K201" t="s" s="2">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="L201" t="s" s="2">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="M201" t="s" s="2">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="N201" t="s" s="2">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="O201" t="s" s="2">
         <v>42</v>
@@ -24646,7 +24652,7 @@
         <v>42</v>
       </c>
       <c r="AE201" t="s" s="2">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="AF201" t="s" s="2">
         <v>40</v>
@@ -24672,7 +24678,7 @@
     </row>
     <row r="202" hidden="true">
       <c r="A202" t="s" s="2">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B202" s="2"/>
       <c r="C202" t="s" s="2">
@@ -24698,16 +24704,16 @@
         <v>135</v>
       </c>
       <c r="K202" t="s" s="2">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="L202" t="s" s="2">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="M202" t="s" s="2">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="N202" t="s" s="2">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="O202" t="s" s="2">
         <v>42</v>
@@ -24735,10 +24741,10 @@
         <v>247</v>
       </c>
       <c r="X202" t="s" s="2">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="Y202" t="s" s="2">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="Z202" t="s" s="2">
         <v>42</v>
@@ -24756,7 +24762,7 @@
         <v>42</v>
       </c>
       <c r="AE202" t="s" s="2">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="AF202" t="s" s="2">
         <v>40</v>
@@ -24782,7 +24788,7 @@
     </row>
     <row r="203" hidden="true">
       <c r="A203" t="s" s="2">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="B203" s="2"/>
       <c r="C203" t="s" s="2">
@@ -24808,16 +24814,16 @@
         <v>135</v>
       </c>
       <c r="K203" t="s" s="2">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="L203" t="s" s="2">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="M203" t="s" s="2">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="N203" t="s" s="2">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="O203" t="s" s="2">
         <v>42</v>
@@ -24845,10 +24851,10 @@
         <v>247</v>
       </c>
       <c r="X203" t="s" s="2">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="Y203" t="s" s="2">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="Z203" t="s" s="2">
         <v>42</v>
@@ -24866,7 +24872,7 @@
         <v>42</v>
       </c>
       <c r="AE203" t="s" s="2">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="AF203" t="s" s="2">
         <v>40</v>
@@ -24892,7 +24898,7 @@
     </row>
     <row r="204" hidden="true">
       <c r="A204" t="s" s="2">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="B204" s="2"/>
       <c r="C204" t="s" s="2">
@@ -24915,19 +24921,19 @@
         <v>42</v>
       </c>
       <c r="J204" t="s" s="2">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="K204" t="s" s="2">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="L204" t="s" s="2">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="M204" t="s" s="2">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="N204" t="s" s="2">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="O204" t="s" s="2">
         <v>42</v>
@@ -24976,7 +24982,7 @@
         <v>42</v>
       </c>
       <c r="AE204" t="s" s="2">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="AF204" t="s" s="2">
         <v>40</v>
@@ -25002,14 +25008,14 @@
     </row>
     <row r="205">
       <c r="A205" t="s" s="2">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="B205" s="2"/>
       <c r="C205" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D205" t="s" s="2">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="E205" t="s" s="2">
         <v>40</v>
@@ -25030,14 +25036,14 @@
         <v>371</v>
       </c>
       <c r="K205" t="s" s="2">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="L205" t="s" s="2">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="M205" s="2"/>
       <c r="N205" t="s" s="2">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="O205" t="s" s="2">
         <v>42</v>
@@ -25086,7 +25092,7 @@
         <v>42</v>
       </c>
       <c r="AE205" t="s" s="2">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="AF205" t="s" s="2">
         <v>40</v>
@@ -25112,7 +25118,7 @@
     </row>
     <row r="206" hidden="true">
       <c r="A206" t="s" s="2">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="B206" s="2"/>
       <c r="C206" t="s" s="2">
@@ -25218,7 +25224,7 @@
     </row>
     <row r="207" hidden="true">
       <c r="A207" t="s" s="2">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="B207" s="2"/>
       <c r="C207" t="s" s="2">
@@ -25326,7 +25332,7 @@
     </row>
     <row r="208" hidden="true">
       <c r="A208" t="s" s="2">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="B208" s="2"/>
       <c r="C208" t="s" s="2">
@@ -25436,7 +25442,7 @@
     </row>
     <row r="209">
       <c r="A209" t="s" s="2">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="B209" s="2"/>
       <c r="C209" t="s" s="2">
@@ -25467,13 +25473,13 @@
         <v>388</v>
       </c>
       <c r="L209" t="s" s="2">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="M209" t="s" s="2">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="N209" t="s" s="2">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="O209" t="s" s="2">
         <v>42</v>
@@ -25522,7 +25528,7 @@
         <v>42</v>
       </c>
       <c r="AE209" t="s" s="2">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="AF209" t="s" s="2">
         <v>40</v>
@@ -25548,7 +25554,7 @@
     </row>
     <row r="210" hidden="true">
       <c r="A210" t="s" s="2">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="B210" s="2"/>
       <c r="C210" t="s" s="2">
@@ -25574,14 +25580,14 @@
         <v>69</v>
       </c>
       <c r="K210" t="s" s="2">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="L210" t="s" s="2">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="M210" s="2"/>
       <c r="N210" t="s" s="2">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="O210" t="s" s="2">
         <v>42</v>
@@ -25609,10 +25615,10 @@
         <v>129</v>
       </c>
       <c r="X210" t="s" s="2">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="Y210" t="s" s="2">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="Z210" t="s" s="2">
         <v>42</v>
@@ -25630,7 +25636,7 @@
         <v>42</v>
       </c>
       <c r="AE210" t="s" s="2">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="AF210" t="s" s="2">
         <v>40</v>
@@ -25656,14 +25662,14 @@
     </row>
     <row r="211">
       <c r="A211" t="s" s="2">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="B211" s="2"/>
       <c r="C211" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D211" t="s" s="2">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="E211" t="s" s="2">
         <v>50</v>
@@ -25684,14 +25690,14 @@
         <v>52</v>
       </c>
       <c r="K211" t="s" s="2">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="L211" t="s" s="2">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="M211" s="2"/>
       <c r="N211" t="s" s="2">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="O211" t="s" s="2">
         <v>42</v>
@@ -25740,7 +25746,7 @@
         <v>42</v>
       </c>
       <c r="AE211" t="s" s="2">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="AF211" t="s" s="2">
         <v>50</v>
@@ -25766,7 +25772,7 @@
     </row>
     <row r="212" hidden="true">
       <c r="A212" t="s" s="2">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="B212" s="2"/>
       <c r="C212" t="s" s="2">
@@ -25792,16 +25798,16 @@
         <v>135</v>
       </c>
       <c r="K212" t="s" s="2">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="L212" t="s" s="2">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="M212" t="s" s="2">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="N212" t="s" s="2">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="O212" t="s" s="2">
         <v>42</v>
@@ -25850,7 +25856,7 @@
         <v>42</v>
       </c>
       <c r="AE212" t="s" s="2">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="AF212" t="s" s="2">
         <v>40</v>
@@ -25876,7 +25882,7 @@
     </row>
     <row r="213" hidden="true">
       <c r="A213" t="s" s="2">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="B213" s="2"/>
       <c r="C213" t="s" s="2">
@@ -25899,19 +25905,19 @@
         <v>42</v>
       </c>
       <c r="J213" t="s" s="2">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="K213" t="s" s="2">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="L213" t="s" s="2">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="M213" t="s" s="2">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="N213" t="s" s="2">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="O213" t="s" s="2">
         <v>42</v>
@@ -25960,7 +25966,7 @@
         <v>42</v>
       </c>
       <c r="AE213" t="s" s="2">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="AF213" t="s" s="2">
         <v>40</v>
@@ -25986,7 +25992,7 @@
     </row>
     <row r="214">
       <c r="A214" t="s" s="2">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="B214" s="2"/>
       <c r="C214" t="s" s="2">
@@ -26012,16 +26018,16 @@
         <v>371</v>
       </c>
       <c r="K214" t="s" s="2">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="L214" t="s" s="2">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="M214" t="s" s="2">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="N214" t="s" s="2">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="O214" t="s" s="2">
         <v>42</v>
@@ -26070,7 +26076,7 @@
         <v>42</v>
       </c>
       <c r="AE214" t="s" s="2">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="AF214" t="s" s="2">
         <v>40</v>
@@ -26091,12 +26097,12 @@
         <v>42</v>
       </c>
       <c r="AL214" t="s" s="2">
-        <v>790</v>
+        <v>792</v>
       </c>
     </row>
     <row r="215" hidden="true">
       <c r="A215" t="s" s="2">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="B215" s="2"/>
       <c r="C215" t="s" s="2">
@@ -26202,7 +26208,7 @@
     </row>
     <row r="216" hidden="true">
       <c r="A216" t="s" s="2">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="B216" s="2"/>
       <c r="C216" t="s" s="2">
@@ -26310,7 +26316,7 @@
     </row>
     <row r="217" hidden="true">
       <c r="A217" t="s" s="2">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B217" s="2"/>
       <c r="C217" t="s" s="2">
@@ -26420,7 +26426,7 @@
     </row>
     <row r="218">
       <c r="A218" t="s" s="2">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="B218" s="2"/>
       <c r="C218" t="s" s="2">
@@ -26446,14 +26452,14 @@
         <v>383</v>
       </c>
       <c r="K218" t="s" s="2">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="L218" t="s" s="2">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="M218" s="2"/>
       <c r="N218" t="s" s="2">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="O218" t="s" s="2">
         <v>42</v>
@@ -26502,7 +26508,7 @@
         <v>42</v>
       </c>
       <c r="AE218" t="s" s="2">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="AF218" t="s" s="2">
         <v>50</v>
@@ -26528,7 +26534,7 @@
     </row>
     <row r="219">
       <c r="A219" t="s" s="2">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="B219" s="2"/>
       <c r="C219" t="s" s="2">
@@ -26554,16 +26560,16 @@
         <v>229</v>
       </c>
       <c r="K219" t="s" s="2">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="L219" t="s" s="2">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="M219" t="s" s="2">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="N219" t="s" s="2">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="O219" t="s" s="2">
         <v>42</v>
@@ -26612,7 +26618,7 @@
         <v>42</v>
       </c>
       <c r="AE219" t="s" s="2">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="AF219" t="s" s="2">
         <v>50</v>
@@ -26638,14 +26644,14 @@
     </row>
     <row r="220">
       <c r="A220" t="s" s="2">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="B220" s="2"/>
       <c r="C220" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D220" t="s" s="2">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="E220" t="s" s="2">
         <v>50</v>
@@ -26663,17 +26669,17 @@
         <v>42</v>
       </c>
       <c r="J220" t="s" s="2">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="K220" t="s" s="2">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="L220" t="s" s="2">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="M220" s="2"/>
       <c r="N220" t="s" s="2">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="O220" t="s" s="2">
         <v>42</v>
@@ -26722,7 +26728,7 @@
         <v>42</v>
       </c>
       <c r="AE220" t="s" s="2">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="AF220" t="s" s="2">
         <v>50</v>
@@ -26748,7 +26754,7 @@
     </row>
     <row r="221" hidden="true">
       <c r="A221" t="s" s="2">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="B221" s="2"/>
       <c r="C221" t="s" s="2">
@@ -26774,14 +26780,14 @@
         <v>52</v>
       </c>
       <c r="K221" t="s" s="2">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="L221" t="s" s="2">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="M221" s="2"/>
       <c r="N221" t="s" s="2">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="O221" t="s" s="2">
         <v>42</v>
@@ -26830,7 +26836,7 @@
         <v>42</v>
       </c>
       <c r="AE221" t="s" s="2">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="AF221" t="s" s="2">
         <v>40</v>
@@ -26856,7 +26862,7 @@
     </row>
     <row r="222" hidden="true">
       <c r="A222" t="s" s="2">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="B222" s="2"/>
       <c r="C222" t="s" s="2">
@@ -26879,19 +26885,19 @@
         <v>42</v>
       </c>
       <c r="J222" t="s" s="2">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="K222" t="s" s="2">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="L222" t="s" s="2">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="M222" t="s" s="2">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="N222" t="s" s="2">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="O222" t="s" s="2">
         <v>42</v>
@@ -26940,7 +26946,7 @@
         <v>42</v>
       </c>
       <c r="AE222" t="s" s="2">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="AF222" t="s" s="2">
         <v>40</v>
@@ -26966,14 +26972,14 @@
     </row>
     <row r="223">
       <c r="A223" t="s" s="2">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="B223" s="2"/>
       <c r="C223" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D223" t="s" s="2">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="E223" t="s" s="2">
         <v>40</v>
@@ -26994,16 +27000,16 @@
         <v>371</v>
       </c>
       <c r="K223" t="s" s="2">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="L223" t="s" s="2">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="M223" t="s" s="2">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="N223" t="s" s="2">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="O223" t="s" s="2">
         <v>42</v>
@@ -27052,7 +27058,7 @@
         <v>42</v>
       </c>
       <c r="AE223" t="s" s="2">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="AF223" t="s" s="2">
         <v>40</v>
@@ -27078,7 +27084,7 @@
     </row>
     <row r="224" hidden="true">
       <c r="A224" t="s" s="2">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="B224" s="2"/>
       <c r="C224" t="s" s="2">
@@ -27184,7 +27190,7 @@
     </row>
     <row r="225" hidden="true">
       <c r="A225" t="s" s="2">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="B225" s="2"/>
       <c r="C225" t="s" s="2">
@@ -27292,7 +27298,7 @@
     </row>
     <row r="226" hidden="true">
       <c r="A226" t="s" s="2">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="B226" s="2"/>
       <c r="C226" t="s" s="2">
@@ -27402,7 +27408,7 @@
     </row>
     <row r="227" hidden="true">
       <c r="A227" t="s" s="2">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="B227" s="2"/>
       <c r="C227" t="s" s="2">
@@ -27428,10 +27434,10 @@
         <v>383</v>
       </c>
       <c r="K227" t="s" s="2">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="L227" t="s" s="2">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="M227" s="2"/>
       <c r="N227" t="s" s="2">
@@ -27484,7 +27490,7 @@
         <v>42</v>
       </c>
       <c r="AE227" t="s" s="2">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="AF227" t="s" s="2">
         <v>40</v>
@@ -27510,7 +27516,7 @@
     </row>
     <row r="228" hidden="true">
       <c r="A228" t="s" s="2">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="B228" s="2"/>
       <c r="C228" t="s" s="2">
@@ -27539,7 +27545,7 @@
         <v>482</v>
       </c>
       <c r="L228" t="s" s="2">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="M228" s="2"/>
       <c r="N228" t="s" s="2">
@@ -27592,7 +27598,7 @@
         <v>42</v>
       </c>
       <c r="AE228" t="s" s="2">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="AF228" t="s" s="2">
         <v>40</v>
@@ -27618,7 +27624,7 @@
     </row>
     <row r="229" hidden="true">
       <c r="A229" t="s" s="2">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="B229" s="2"/>
       <c r="C229" t="s" s="2">
@@ -27647,7 +27653,7 @@
         <v>486</v>
       </c>
       <c r="L229" t="s" s="2">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="M229" s="2"/>
       <c r="N229" t="s" s="2">
@@ -27700,7 +27706,7 @@
         <v>42</v>
       </c>
       <c r="AE229" t="s" s="2">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="AF229" t="s" s="2">
         <v>40</v>
@@ -27726,14 +27732,14 @@
     </row>
     <row r="230">
       <c r="A230" t="s" s="2">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="B230" s="2"/>
       <c r="C230" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D230" t="s" s="2">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="E230" t="s" s="2">
         <v>50</v>
@@ -27754,14 +27760,14 @@
         <v>135</v>
       </c>
       <c r="K230" t="s" s="2">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="L230" t="s" s="2">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="M230" s="2"/>
       <c r="N230" t="s" s="2">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="O230" t="s" s="2">
         <v>42</v>
@@ -27789,7 +27795,7 @@
         <v>129</v>
       </c>
       <c r="X230" t="s" s="2">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="Y230" t="s" s="2">
         <v>42</v>
@@ -27810,7 +27816,7 @@
         <v>42</v>
       </c>
       <c r="AE230" t="s" s="2">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="AF230" t="s" s="2">
         <v>50</v>
@@ -27836,7 +27842,7 @@
     </row>
     <row r="231" hidden="true">
       <c r="A231" t="s" s="2">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="B231" s="2"/>
       <c r="C231" t="s" s="2">
@@ -27942,7 +27948,7 @@
     </row>
     <row r="232" hidden="true">
       <c r="A232" t="s" s="2">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="B232" s="2"/>
       <c r="C232" t="s" s="2">
@@ -28050,7 +28056,7 @@
     </row>
     <row r="233">
       <c r="A233" t="s" s="2">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="B233" s="2"/>
       <c r="C233" t="s" s="2">
@@ -28160,7 +28166,7 @@
     </row>
     <row r="234" hidden="true">
       <c r="A234" t="s" s="2">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="B234" s="2"/>
       <c r="C234" t="s" s="2">
@@ -28266,7 +28272,7 @@
     </row>
     <row r="235" hidden="true">
       <c r="A235" t="s" s="2">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="B235" s="2"/>
       <c r="C235" t="s" s="2">
@@ -28374,7 +28380,7 @@
     </row>
     <row r="236">
       <c r="A236" t="s" s="2">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="B236" s="2"/>
       <c r="C236" t="s" s="2">
@@ -28484,7 +28490,7 @@
     </row>
     <row r="237" hidden="true">
       <c r="A237" t="s" s="2">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="B237" s="2"/>
       <c r="C237" t="s" s="2">
@@ -28592,14 +28598,14 @@
     </row>
     <row r="238">
       <c r="A238" t="s" s="2">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="B238" s="2"/>
       <c r="C238" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D238" t="s" s="2">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="E238" t="s" s="2">
         <v>50</v>
@@ -28620,7 +28626,7 @@
         <v>69</v>
       </c>
       <c r="K238" t="s" s="2">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="L238" t="s" s="2">
         <v>218</v>
@@ -28702,7 +28708,7 @@
     </row>
     <row r="239">
       <c r="A239" t="s" s="2">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="B239" s="2"/>
       <c r="C239" t="s" s="2">
@@ -28810,7 +28816,7 @@
     </row>
     <row r="240" hidden="true">
       <c r="A240" t="s" s="2">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="B240" s="2"/>
       <c r="C240" t="s" s="2">
@@ -28920,14 +28926,14 @@
     </row>
     <row r="241">
       <c r="A241" t="s" s="2">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="B241" s="2"/>
       <c r="C241" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D241" t="s" s="2">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="E241" t="s" s="2">
         <v>40</v>
@@ -28948,10 +28954,10 @@
         <v>52</v>
       </c>
       <c r="K241" t="s" s="2">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="L241" t="s" s="2">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="M241" t="s" s="2">
         <v>239</v>

</xml_diff>

<commit_message>
Refined terminology assets, other
Added code system with new coupon coverage-class concepts and new value set to add them to the current HL7 coverage-class values. Added placeholder code systems for multiple NCPDP and other code/identifier systems for which HL7/FHIR URLs are not available–to be replaced with HL7-maintained URLs or NamingSystem resources within this IG (when supported by the publishing process); see Terminology page. Added state/province and constrained country value sets and related element bindings in Patient and pharmacy Organization profiles. Added currency bindings in ClaimResponse cost elements. Refined content and layout on terminology, code system, value set and naming system pages. Refined business error content in ClaimResponse and clarified related guidance in the Error Handling page. Refined content on the Consumer vs Provider RTPBC page.
</commit_message>
<xml_diff>
--- a/output/carin-rtpbc-ClaimResponse.xlsx
+++ b/output/carin-rtpbc-ClaimResponse.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8317" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8317" uniqueCount="863">
   <si>
     <t>Path</t>
   </si>
@@ -1357,6 +1357,9 @@
     <t>Currencies</t>
   </si>
   <si>
+    <t>http://hl7.org/fhir/ValueSet/currencies</t>
+  </si>
+  <si>
     <t>Money.currency</t>
   </si>
   <si>
@@ -1823,10 +1826,10 @@
     <t>There are many representations for units of measure and in many contexts, particular representations are fixed and required. I.e. mcg for micrograms.</t>
   </si>
   <si>
-    <t>Billing quantity unity of measure</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/carin/ValueSet/rtpbc-billing-units</t>
+    <t>Billing quantity unit of measure</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/carin/ValueSet/rtpbc-billing-unit</t>
   </si>
   <si>
     <t>Quantity.unit</t>
@@ -2411,6 +2414,12 @@
     <t>Required to provide human readable explanation.</t>
   </si>
   <si>
+    <t>RTPBC Coverage Summary</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/carin/ValueSet/rtpbc-coverage-summary</t>
+  </si>
+  <si>
     <t>ClaimResponse.processNote.language</t>
   </si>
   <si>
@@ -2603,7 +2612,10 @@
     <t>Required to convey processing errors.</t>
   </si>
   <si>
-    <t>RTPBC Reject Codes (to be determined. Correspond to NCPDP 511-FB)</t>
+    <t>RTPBC Error Codes</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/carin/ValueSet/rtpbc-error-code</t>
   </si>
   <si>
     <t>ClaimResponse.error.code.id</t>
@@ -12485,7 +12497,7 @@
         <v>431</v>
       </c>
       <c r="Y89" t="s" s="2">
-        <v>42</v>
+        <v>432</v>
       </c>
       <c r="Z89" t="s" s="2">
         <v>42</v>
@@ -12503,7 +12515,7 @@
         <v>42</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>40</v>
@@ -12529,7 +12541,7 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -12555,16 +12567,16 @@
         <v>422</v>
       </c>
       <c r="K90" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N90" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="O90" t="s" s="2">
         <v>42</v>
@@ -12613,7 +12625,7 @@
         <v>42</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AF90" t="s" s="2">
         <v>40</v>
@@ -12639,7 +12651,7 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s" s="2">
@@ -12665,14 +12677,14 @@
         <v>371</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="M91" s="2"/>
       <c r="N91" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="O91" t="s" s="2">
         <v>42</v>
@@ -12721,7 +12733,7 @@
         <v>42</v>
       </c>
       <c r="AE91" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="AF91" t="s" s="2">
         <v>40</v>
@@ -12747,7 +12759,7 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s" s="2">
@@ -12853,7 +12865,7 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" t="s" s="2">
@@ -12961,7 +12973,7 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" t="s" s="2">
@@ -13071,7 +13083,7 @@
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" t="s" s="2">
@@ -13097,14 +13109,14 @@
         <v>383</v>
       </c>
       <c r="K95" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="M95" s="2"/>
       <c r="N95" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="O95" t="s" s="2">
         <v>42</v>
@@ -13153,7 +13165,7 @@
         <v>42</v>
       </c>
       <c r="AE95" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="AF95" t="s" s="2">
         <v>50</v>
@@ -13179,7 +13191,7 @@
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" t="s" s="2">
@@ -13205,10 +13217,10 @@
         <v>383</v>
       </c>
       <c r="K96" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="L96" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="M96" s="2"/>
       <c r="N96" t="s" s="2">
@@ -13261,7 +13273,7 @@
         <v>42</v>
       </c>
       <c r="AE96" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AF96" t="s" s="2">
         <v>40</v>
@@ -13287,7 +13299,7 @@
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" t="s" s="2">
@@ -13313,10 +13325,10 @@
         <v>42</v>
       </c>
       <c r="K97" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="L97" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
@@ -13367,7 +13379,7 @@
         <v>42</v>
       </c>
       <c r="AE97" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AF97" t="s" s="2">
         <v>50</v>
@@ -13393,7 +13405,7 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" t="s" s="2">
@@ -13419,14 +13431,14 @@
         <v>371</v>
       </c>
       <c r="K98" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="L98" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="M98" s="2"/>
       <c r="N98" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="O98" t="s" s="2">
         <v>42</v>
@@ -13475,7 +13487,7 @@
         <v>42</v>
       </c>
       <c r="AE98" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AF98" t="s" s="2">
         <v>40</v>
@@ -13501,7 +13513,7 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" t="s" s="2">
@@ -13607,7 +13619,7 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
@@ -13715,7 +13727,7 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -13825,7 +13837,7 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
@@ -13851,14 +13863,14 @@
         <v>383</v>
       </c>
       <c r="K102" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="M102" s="2"/>
       <c r="N102" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="O102" t="s" s="2">
         <v>42</v>
@@ -13907,7 +13919,7 @@
         <v>42</v>
       </c>
       <c r="AE102" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="AF102" t="s" s="2">
         <v>50</v>
@@ -13933,7 +13945,7 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
@@ -13959,10 +13971,10 @@
         <v>383</v>
       </c>
       <c r="K103" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="L103" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="M103" s="2"/>
       <c r="N103" t="s" s="2">
@@ -14015,7 +14027,7 @@
         <v>42</v>
       </c>
       <c r="AE103" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="AF103" t="s" s="2">
         <v>40</v>
@@ -14041,7 +14053,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -14067,10 +14079,10 @@
         <v>42</v>
       </c>
       <c r="K104" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="L104" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M104" s="2"/>
       <c r="N104" s="2"/>
@@ -14121,7 +14133,7 @@
         <v>42</v>
       </c>
       <c r="AE104" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="AF104" t="s" s="2">
         <v>40</v>
@@ -14147,7 +14159,7 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
@@ -14173,14 +14185,14 @@
         <v>371</v>
       </c>
       <c r="K105" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="L105" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="M105" s="2"/>
       <c r="N105" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="O105" t="s" s="2">
         <v>42</v>
@@ -14229,7 +14241,7 @@
         <v>42</v>
       </c>
       <c r="AE105" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="AF105" t="s" s="2">
         <v>40</v>
@@ -14255,7 +14267,7 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
@@ -14361,7 +14373,7 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -14387,10 +14399,10 @@
         <v>95</v>
       </c>
       <c r="K107" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="L107" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="M107" s="2"/>
       <c r="N107" s="2"/>
@@ -14465,10 +14477,10 @@
     </row>
     <row r="108">
       <c r="A108" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B108" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C108" t="s" s="2">
         <v>42</v>
@@ -14493,13 +14505,13 @@
         <v>95</v>
       </c>
       <c r="K108" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="L108" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="M108" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="N108" s="2"/>
       <c r="O108" t="s" s="2">
@@ -14575,7 +14587,7 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
@@ -14685,14 +14697,14 @@
     </row>
     <row r="110">
       <c r="A110" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D110" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="E110" t="s" s="2">
         <v>50</v>
@@ -14713,16 +14725,16 @@
         <v>383</v>
       </c>
       <c r="K110" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="L110" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="M110" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="N110" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="O110" t="s" s="2">
         <v>42</v>
@@ -14771,7 +14783,7 @@
         <v>42</v>
       </c>
       <c r="AE110" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="AF110" t="s" s="2">
         <v>40</v>
@@ -14797,7 +14809,7 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" t="s" s="2">
@@ -14823,14 +14835,14 @@
         <v>383</v>
       </c>
       <c r="K111" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="L111" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="M111" s="2"/>
       <c r="N111" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="O111" t="s" s="2">
         <v>42</v>
@@ -14879,7 +14891,7 @@
         <v>42</v>
       </c>
       <c r="AE111" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="AF111" t="s" s="2">
         <v>40</v>
@@ -14905,7 +14917,7 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
@@ -14931,14 +14943,14 @@
         <v>383</v>
       </c>
       <c r="K112" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="L112" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="M112" s="2"/>
       <c r="N112" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="O112" t="s" s="2">
         <v>42</v>
@@ -14987,7 +14999,7 @@
         <v>42</v>
       </c>
       <c r="AE112" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="AF112" t="s" s="2">
         <v>40</v>
@@ -15013,14 +15025,14 @@
     </row>
     <row r="113">
       <c r="A113" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D113" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E113" t="s" s="2">
         <v>50</v>
@@ -15038,17 +15050,17 @@
         <v>42</v>
       </c>
       <c r="J113" t="s" s="2">
+        <v>497</v>
+      </c>
+      <c r="K113" t="s" s="2">
         <v>496</v>
       </c>
-      <c r="K113" t="s" s="2">
-        <v>495</v>
-      </c>
       <c r="L113" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="M113" s="2"/>
       <c r="N113" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="O113" t="s" s="2">
         <v>42</v>
@@ -15097,7 +15109,7 @@
         <v>42</v>
       </c>
       <c r="AE113" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="AF113" t="s" s="2">
         <v>40</v>
@@ -15123,7 +15135,7 @@
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" t="s" s="2">
@@ -15229,7 +15241,7 @@
     </row>
     <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" t="s" s="2">
@@ -15337,14 +15349,14 @@
     </row>
     <row r="116">
       <c r="A116" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D116" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="E116" t="s" s="2">
         <v>50</v>
@@ -15365,7 +15377,7 @@
         <v>52</v>
       </c>
       <c r="K116" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="L116" t="s" s="2">
         <v>281</v>
@@ -15447,7 +15459,7 @@
     </row>
     <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" t="s" s="2">
@@ -15555,7 +15567,7 @@
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" t="s" s="2">
@@ -15663,7 +15675,7 @@
     </row>
     <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" t="s" s="2">
@@ -15771,14 +15783,14 @@
     </row>
     <row r="120">
       <c r="A120" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D120" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="E120" t="s" s="2">
         <v>50</v>
@@ -15799,16 +15811,16 @@
         <v>135</v>
       </c>
       <c r="K120" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="L120" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="M120" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="N120" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="O120" t="s" s="2">
         <v>42</v>
@@ -15836,10 +15848,10 @@
         <v>129</v>
       </c>
       <c r="X120" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="Y120" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="Z120" t="s" s="2">
         <v>42</v>
@@ -15857,7 +15869,7 @@
         <v>42</v>
       </c>
       <c r="AE120" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="AF120" t="s" s="2">
         <v>50</v>
@@ -15883,7 +15895,7 @@
     </row>
     <row r="121" hidden="true">
       <c r="A121" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B121" s="2"/>
       <c r="C121" t="s" s="2">
@@ -15989,7 +16001,7 @@
     </row>
     <row r="122" hidden="true">
       <c r="A122" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" t="s" s="2">
@@ -16097,7 +16109,7 @@
     </row>
     <row r="123">
       <c r="A123" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" t="s" s="2">
@@ -16207,7 +16219,7 @@
     </row>
     <row r="124" hidden="true">
       <c r="A124" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" t="s" s="2">
@@ -16313,7 +16325,7 @@
     </row>
     <row r="125" hidden="true">
       <c r="A125" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" t="s" s="2">
@@ -16421,7 +16433,7 @@
     </row>
     <row r="126">
       <c r="A126" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" t="s" s="2">
@@ -16531,7 +16543,7 @@
     </row>
     <row r="127" hidden="true">
       <c r="A127" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" t="s" s="2">
@@ -16639,7 +16651,7 @@
     </row>
     <row r="128">
       <c r="A128" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" t="s" s="2">
@@ -16747,14 +16759,14 @@
     </row>
     <row r="129">
       <c r="A129" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D129" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E129" t="s" s="2">
         <v>50</v>
@@ -16775,10 +16787,10 @@
         <v>52</v>
       </c>
       <c r="K129" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="L129" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="M129" s="2"/>
       <c r="N129" t="s" s="2">
@@ -16857,7 +16869,7 @@
     </row>
     <row r="130" hidden="true">
       <c r="A130" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" t="s" s="2">
@@ -16967,7 +16979,7 @@
     </row>
     <row r="131" hidden="true">
       <c r="A131" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B131" s="2"/>
       <c r="C131" t="s" s="2">
@@ -17077,7 +17089,7 @@
     </row>
     <row r="132" hidden="true">
       <c r="A132" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B132" s="2"/>
       <c r="C132" t="s" s="2">
@@ -17103,16 +17115,16 @@
         <v>135</v>
       </c>
       <c r="K132" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="L132" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="M132" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="N132" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="O132" t="s" s="2">
         <v>42</v>
@@ -17140,10 +17152,10 @@
         <v>247</v>
       </c>
       <c r="X132" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="Y132" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="Z132" t="s" s="2">
         <v>42</v>
@@ -17161,7 +17173,7 @@
         <v>42</v>
       </c>
       <c r="AE132" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="AF132" t="s" s="2">
         <v>40</v>
@@ -17182,12 +17194,12 @@
         <v>42</v>
       </c>
       <c r="AL132" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="133" hidden="true">
       <c r="A133" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B133" s="2"/>
       <c r="C133" t="s" s="2">
@@ -17213,16 +17225,16 @@
         <v>135</v>
       </c>
       <c r="K133" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="L133" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="M133" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="N133" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="O133" t="s" s="2">
         <v>42</v>
@@ -17250,10 +17262,10 @@
         <v>247</v>
       </c>
       <c r="X133" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="Y133" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="Z133" t="s" s="2">
         <v>42</v>
@@ -17271,7 +17283,7 @@
         <v>42</v>
       </c>
       <c r="AE133" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="AF133" t="s" s="2">
         <v>40</v>
@@ -17292,12 +17304,12 @@
         <v>42</v>
       </c>
       <c r="AL133" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="134" hidden="true">
       <c r="A134" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" t="s" s="2">
@@ -17320,17 +17332,17 @@
         <v>42</v>
       </c>
       <c r="J134" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="K134" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="L134" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="M134" s="2"/>
       <c r="N134" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="O134" t="s" s="2">
         <v>42</v>
@@ -17379,7 +17391,7 @@
         <v>42</v>
       </c>
       <c r="AE134" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="AF134" t="s" s="2">
         <v>40</v>
@@ -17397,15 +17409,15 @@
         <v>42</v>
       </c>
       <c r="AK134" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="AL134" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="135" hidden="true">
       <c r="A135" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" t="s" s="2">
@@ -17428,17 +17440,17 @@
         <v>42</v>
       </c>
       <c r="J135" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="K135" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="L135" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="M135" s="2"/>
       <c r="N135" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="O135" t="s" s="2">
         <v>42</v>
@@ -17466,10 +17478,10 @@
         <v>247</v>
       </c>
       <c r="X135" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="Y135" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="Z135" t="s" s="2">
         <v>42</v>
@@ -17487,7 +17499,7 @@
         <v>42</v>
       </c>
       <c r="AE135" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="AF135" t="s" s="2">
         <v>40</v>
@@ -17505,22 +17517,22 @@
         <v>42</v>
       </c>
       <c r="AK135" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="AL135" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D136" t="s" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E136" t="s" s="2">
         <v>50</v>
@@ -17538,17 +17550,17 @@
         <v>42</v>
       </c>
       <c r="J136" t="s" s="2">
+        <v>561</v>
+      </c>
+      <c r="K136" t="s" s="2">
         <v>560</v>
       </c>
-      <c r="K136" t="s" s="2">
-        <v>559</v>
-      </c>
       <c r="L136" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="M136" s="2"/>
       <c r="N136" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="O136" t="s" s="2">
         <v>42</v>
@@ -17597,7 +17609,7 @@
         <v>42</v>
       </c>
       <c r="AE136" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="AF136" t="s" s="2">
         <v>40</v>
@@ -17618,12 +17630,12 @@
         <v>42</v>
       </c>
       <c r="AL136" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="137" hidden="true">
       <c r="A137" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B137" s="2"/>
       <c r="C137" t="s" s="2">
@@ -17729,7 +17741,7 @@
     </row>
     <row r="138" hidden="true">
       <c r="A138" t="s" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B138" s="2"/>
       <c r="C138" t="s" s="2">
@@ -17837,14 +17849,14 @@
     </row>
     <row r="139">
       <c r="A139" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B139" s="2"/>
       <c r="C139" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D139" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="E139" t="s" s="2">
         <v>50</v>
@@ -17865,16 +17877,16 @@
         <v>422</v>
       </c>
       <c r="K139" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="L139" t="s" s="2">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="M139" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="N139" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="O139" t="s" s="2">
         <v>42</v>
@@ -17923,7 +17935,7 @@
         <v>42</v>
       </c>
       <c r="AE139" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="AF139" t="s" s="2">
         <v>40</v>
@@ -17944,12 +17956,12 @@
         <v>42</v>
       </c>
       <c r="AL139" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="140" hidden="true">
       <c r="A140" t="s" s="2">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" t="s" s="2">
@@ -17975,20 +17987,20 @@
         <v>69</v>
       </c>
       <c r="K140" t="s" s="2">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="L140" t="s" s="2">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="M140" s="2"/>
       <c r="N140" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="O140" t="s" s="2">
         <v>42</v>
       </c>
       <c r="P140" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="Q140" t="s" s="2">
         <v>42</v>
@@ -18012,10 +18024,10 @@
         <v>129</v>
       </c>
       <c r="X140" t="s" s="2">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="Y140" t="s" s="2">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="Z140" t="s" s="2">
         <v>42</v>
@@ -18033,7 +18045,7 @@
         <v>42</v>
       </c>
       <c r="AE140" t="s" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="AF140" t="s" s="2">
         <v>40</v>
@@ -18054,19 +18066,19 @@
         <v>42</v>
       </c>
       <c r="AL140" t="s" s="2">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s" s="2">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D141" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="E141" t="s" s="2">
         <v>50</v>
@@ -18087,14 +18099,14 @@
         <v>52</v>
       </c>
       <c r="K141" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="L141" t="s" s="2">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="M141" s="2"/>
       <c r="N141" t="s" s="2">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="O141" t="s" s="2">
         <v>42</v>
@@ -18122,10 +18134,10 @@
         <v>129</v>
       </c>
       <c r="X141" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="Y141" t="s" s="2">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="Z141" t="s" s="2">
         <v>42</v>
@@ -18143,7 +18155,7 @@
         <v>42</v>
       </c>
       <c r="AE141" t="s" s="2">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="AF141" t="s" s="2">
         <v>40</v>
@@ -18164,12 +18176,12 @@
         <v>42</v>
       </c>
       <c r="AL141" t="s" s="2">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="142" hidden="true">
       <c r="A142" t="s" s="2">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" t="s" s="2">
@@ -18195,14 +18207,14 @@
         <v>63</v>
       </c>
       <c r="K142" t="s" s="2">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="L142" t="s" s="2">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="M142" s="2"/>
       <c r="N142" t="s" s="2">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="O142" t="s" s="2">
         <v>42</v>
@@ -18251,7 +18263,7 @@
         <v>42</v>
       </c>
       <c r="AE142" t="s" s="2">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="AF142" t="s" s="2">
         <v>40</v>
@@ -18260,7 +18272,7 @@
         <v>50</v>
       </c>
       <c r="AH142" t="s" s="2">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="AI142" t="s" s="2">
         <v>61</v>
@@ -18272,12 +18284,12 @@
         <v>42</v>
       </c>
       <c r="AL142" t="s" s="2">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="143" hidden="true">
       <c r="A143" t="s" s="2">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" t="s" s="2">
@@ -18303,16 +18315,16 @@
         <v>69</v>
       </c>
       <c r="K143" t="s" s="2">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="L143" t="s" s="2">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="M143" t="s" s="2">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="N143" t="s" s="2">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="O143" t="s" s="2">
         <v>42</v>
@@ -18361,7 +18373,7 @@
         <v>42</v>
       </c>
       <c r="AE143" t="s" s="2">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="AF143" t="s" s="2">
         <v>40</v>
@@ -18382,12 +18394,12 @@
         <v>42</v>
       </c>
       <c r="AL143" t="s" s="2">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="144" hidden="true">
       <c r="A144" t="s" s="2">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" t="s" s="2">
@@ -18413,14 +18425,14 @@
         <v>414</v>
       </c>
       <c r="K144" t="s" s="2">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="L144" t="s" s="2">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="M144" s="2"/>
       <c r="N144" t="s" s="2">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="O144" t="s" s="2">
         <v>42</v>
@@ -18469,7 +18481,7 @@
         <v>42</v>
       </c>
       <c r="AE144" t="s" s="2">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="AF144" t="s" s="2">
         <v>40</v>
@@ -18495,7 +18507,7 @@
     </row>
     <row r="145" hidden="true">
       <c r="A145" t="s" s="2">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" t="s" s="2">
@@ -18521,16 +18533,16 @@
         <v>422</v>
       </c>
       <c r="K145" t="s" s="2">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="L145" t="s" s="2">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="M145" t="s" s="2">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="N145" t="s" s="2">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="O145" t="s" s="2">
         <v>42</v>
@@ -18579,7 +18591,7 @@
         <v>42</v>
       </c>
       <c r="AE145" t="s" s="2">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="AF145" t="s" s="2">
         <v>40</v>
@@ -18605,7 +18617,7 @@
     </row>
     <row r="146" hidden="true">
       <c r="A146" t="s" s="2">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" t="s" s="2">
@@ -18631,16 +18643,16 @@
         <v>414</v>
       </c>
       <c r="K146" t="s" s="2">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="L146" t="s" s="2">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="M146" t="s" s="2">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="N146" t="s" s="2">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="O146" t="s" s="2">
         <v>42</v>
@@ -18689,7 +18701,7 @@
         <v>42</v>
       </c>
       <c r="AE146" t="s" s="2">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="AF146" t="s" s="2">
         <v>40</v>
@@ -18710,12 +18722,12 @@
         <v>42</v>
       </c>
       <c r="AL146" t="s" s="2">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="147" hidden="true">
       <c r="A147" t="s" s="2">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" t="s" s="2">
@@ -18741,16 +18753,16 @@
         <v>135</v>
       </c>
       <c r="K147" t="s" s="2">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="L147" t="s" s="2">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="M147" t="s" s="2">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="N147" t="s" s="2">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="O147" t="s" s="2">
         <v>42</v>
@@ -18778,10 +18790,10 @@
         <v>247</v>
       </c>
       <c r="X147" t="s" s="2">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="Y147" t="s" s="2">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="Z147" t="s" s="2">
         <v>42</v>
@@ -18799,7 +18811,7 @@
         <v>42</v>
       </c>
       <c r="AE147" t="s" s="2">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="AF147" t="s" s="2">
         <v>40</v>
@@ -18825,7 +18837,7 @@
     </row>
     <row r="148" hidden="true">
       <c r="A148" t="s" s="2">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" t="s" s="2">
@@ -18851,14 +18863,14 @@
         <v>135</v>
       </c>
       <c r="K148" t="s" s="2">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="L148" t="s" s="2">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="M148" s="2"/>
       <c r="N148" t="s" s="2">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="O148" t="s" s="2">
         <v>42</v>
@@ -18886,10 +18898,10 @@
         <v>247</v>
       </c>
       <c r="X148" t="s" s="2">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="Y148" t="s" s="2">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="Z148" t="s" s="2">
         <v>42</v>
@@ -18907,7 +18919,7 @@
         <v>42</v>
       </c>
       <c r="AE148" t="s" s="2">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="AF148" t="s" s="2">
         <v>40</v>
@@ -18933,7 +18945,7 @@
     </row>
     <row r="149">
       <c r="A149" t="s" s="2">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B149" s="2"/>
       <c r="C149" t="s" s="2">
@@ -19017,7 +19029,7 @@
         <v>42</v>
       </c>
       <c r="AE149" t="s" s="2">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="AF149" t="s" s="2">
         <v>40</v>
@@ -19043,14 +19055,14 @@
     </row>
     <row r="150">
       <c r="A150" t="s" s="2">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D150" t="s" s="2">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="E150" t="s" s="2">
         <v>50</v>
@@ -19071,10 +19083,10 @@
         <v>371</v>
       </c>
       <c r="K150" t="s" s="2">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="L150" t="s" s="2">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="M150" s="2"/>
       <c r="N150" s="2"/>
@@ -19125,7 +19137,7 @@
         <v>42</v>
       </c>
       <c r="AE150" t="s" s="2">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="AF150" t="s" s="2">
         <v>50</v>
@@ -19151,7 +19163,7 @@
     </row>
     <row r="151" hidden="true">
       <c r="A151" t="s" s="2">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B151" s="2"/>
       <c r="C151" t="s" s="2">
@@ -19257,7 +19269,7 @@
     </row>
     <row r="152" hidden="true">
       <c r="A152" t="s" s="2">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" t="s" s="2">
@@ -19365,7 +19377,7 @@
     </row>
     <row r="153" hidden="true">
       <c r="A153" t="s" s="2">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B153" s="2"/>
       <c r="C153" t="s" s="2">
@@ -19475,7 +19487,7 @@
     </row>
     <row r="154">
       <c r="A154" t="s" s="2">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B154" s="2"/>
       <c r="C154" t="s" s="2">
@@ -19587,7 +19599,7 @@
     </row>
     <row r="155" hidden="true">
       <c r="A155" t="s" s="2">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B155" s="2"/>
       <c r="C155" t="s" s="2">
@@ -19697,7 +19709,7 @@
     </row>
     <row r="156">
       <c r="A156" t="s" s="2">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" t="s" s="2">
@@ -19809,7 +19821,7 @@
     </row>
     <row r="157" hidden="true">
       <c r="A157" t="s" s="2">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B157" s="2"/>
       <c r="C157" t="s" s="2">
@@ -19915,7 +19927,7 @@
     </row>
     <row r="158" hidden="true">
       <c r="A158" t="s" s="2">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" t="s" s="2">
@@ -20023,7 +20035,7 @@
     </row>
     <row r="159">
       <c r="A159" t="s" s="2">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" t="s" s="2">
@@ -20135,7 +20147,7 @@
     </row>
     <row r="160">
       <c r="A160" t="s" s="2">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" t="s" s="2">
@@ -20201,7 +20213,7 @@
         <v>431</v>
       </c>
       <c r="Y160" t="s" s="2">
-        <v>42</v>
+        <v>432</v>
       </c>
       <c r="Z160" t="s" s="2">
         <v>42</v>
@@ -20219,7 +20231,7 @@
         <v>42</v>
       </c>
       <c r="AE160" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AF160" t="s" s="2">
         <v>40</v>
@@ -20245,7 +20257,7 @@
     </row>
     <row r="161" hidden="true">
       <c r="A161" t="s" s="2">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B161" s="2"/>
       <c r="C161" t="s" s="2">
@@ -20271,16 +20283,16 @@
         <v>422</v>
       </c>
       <c r="K161" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="L161" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="M161" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N161" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="O161" t="s" s="2">
         <v>42</v>
@@ -20329,7 +20341,7 @@
         <v>42</v>
       </c>
       <c r="AE161" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AF161" t="s" s="2">
         <v>40</v>
@@ -20355,7 +20367,7 @@
     </row>
     <row r="162" hidden="true">
       <c r="A162" t="s" s="2">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" t="s" s="2">
@@ -20381,10 +20393,10 @@
         <v>371</v>
       </c>
       <c r="K162" t="s" s="2">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="L162" t="s" s="2">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="M162" s="2"/>
       <c r="N162" s="2"/>
@@ -20435,7 +20447,7 @@
         <v>42</v>
       </c>
       <c r="AE162" t="s" s="2">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="AF162" t="s" s="2">
         <v>40</v>
@@ -20461,7 +20473,7 @@
     </row>
     <row r="163" hidden="true">
       <c r="A163" t="s" s="2">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" t="s" s="2">
@@ -20567,7 +20579,7 @@
     </row>
     <row r="164" hidden="true">
       <c r="A164" t="s" s="2">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B164" s="2"/>
       <c r="C164" t="s" s="2">
@@ -20675,7 +20687,7 @@
     </row>
     <row r="165" hidden="true">
       <c r="A165" t="s" s="2">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" t="s" s="2">
@@ -20785,7 +20797,7 @@
     </row>
     <row r="166" hidden="true">
       <c r="A166" t="s" s="2">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B166" s="2"/>
       <c r="C166" t="s" s="2">
@@ -20811,16 +20823,16 @@
         <v>135</v>
       </c>
       <c r="K166" t="s" s="2">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="L166" t="s" s="2">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="M166" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="N166" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="O166" t="s" s="2">
         <v>42</v>
@@ -20848,10 +20860,10 @@
         <v>247</v>
       </c>
       <c r="X166" t="s" s="2">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="Y166" t="s" s="2">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="Z166" t="s" s="2">
         <v>42</v>
@@ -20869,7 +20881,7 @@
         <v>42</v>
       </c>
       <c r="AE166" t="s" s="2">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="AF166" t="s" s="2">
         <v>50</v>
@@ -20895,7 +20907,7 @@
     </row>
     <row r="167" hidden="true">
       <c r="A167" t="s" s="2">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" t="s" s="2">
@@ -20921,16 +20933,16 @@
         <v>135</v>
       </c>
       <c r="K167" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="L167" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="M167" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="N167" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="O167" t="s" s="2">
         <v>42</v>
@@ -20958,10 +20970,10 @@
         <v>247</v>
       </c>
       <c r="X167" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="Y167" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="Z167" t="s" s="2">
         <v>42</v>
@@ -20979,7 +20991,7 @@
         <v>42</v>
       </c>
       <c r="AE167" t="s" s="2">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="AF167" t="s" s="2">
         <v>40</v>
@@ -21000,12 +21012,12 @@
         <v>42</v>
       </c>
       <c r="AL167" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="168" hidden="true">
       <c r="A168" t="s" s="2">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B168" s="2"/>
       <c r="C168" t="s" s="2">
@@ -21028,17 +21040,17 @@
         <v>42</v>
       </c>
       <c r="J168" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="K168" t="s" s="2">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="L168" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="M168" s="2"/>
       <c r="N168" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="O168" t="s" s="2">
         <v>42</v>
@@ -21087,7 +21099,7 @@
         <v>42</v>
       </c>
       <c r="AE168" t="s" s="2">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="AF168" t="s" s="2">
         <v>40</v>
@@ -21108,12 +21120,12 @@
         <v>42</v>
       </c>
       <c r="AL168" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="169" hidden="true">
       <c r="A169" t="s" s="2">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" t="s" s="2">
@@ -21139,14 +21151,14 @@
         <v>414</v>
       </c>
       <c r="K169" t="s" s="2">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="L169" t="s" s="2">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="M169" s="2"/>
       <c r="N169" t="s" s="2">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="O169" t="s" s="2">
         <v>42</v>
@@ -21195,7 +21207,7 @@
         <v>42</v>
       </c>
       <c r="AE169" t="s" s="2">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="AF169" t="s" s="2">
         <v>40</v>
@@ -21221,7 +21233,7 @@
     </row>
     <row r="170" hidden="true">
       <c r="A170" t="s" s="2">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B170" s="2"/>
       <c r="C170" t="s" s="2">
@@ -21247,16 +21259,16 @@
         <v>422</v>
       </c>
       <c r="K170" t="s" s="2">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="L170" t="s" s="2">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="M170" t="s" s="2">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="N170" t="s" s="2">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="O170" t="s" s="2">
         <v>42</v>
@@ -21305,7 +21317,7 @@
         <v>42</v>
       </c>
       <c r="AE170" t="s" s="2">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="AF170" t="s" s="2">
         <v>40</v>
@@ -21331,7 +21343,7 @@
     </row>
     <row r="171" hidden="true">
       <c r="A171" t="s" s="2">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B171" s="2"/>
       <c r="C171" t="s" s="2">
@@ -21357,16 +21369,16 @@
         <v>414</v>
       </c>
       <c r="K171" t="s" s="2">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="L171" t="s" s="2">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="M171" t="s" s="2">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="N171" t="s" s="2">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="O171" t="s" s="2">
         <v>42</v>
@@ -21415,7 +21427,7 @@
         <v>42</v>
       </c>
       <c r="AE171" t="s" s="2">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="AF171" t="s" s="2">
         <v>40</v>
@@ -21436,12 +21448,12 @@
         <v>42</v>
       </c>
       <c r="AL171" t="s" s="2">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="172" hidden="true">
       <c r="A172" t="s" s="2">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B172" s="2"/>
       <c r="C172" t="s" s="2">
@@ -21467,10 +21479,10 @@
         <v>383</v>
       </c>
       <c r="K172" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="L172" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="M172" s="2"/>
       <c r="N172" t="s" s="2">
@@ -21523,7 +21535,7 @@
         <v>42</v>
       </c>
       <c r="AE172" t="s" s="2">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="AF172" t="s" s="2">
         <v>40</v>
@@ -21549,7 +21561,7 @@
     </row>
     <row r="173" hidden="true">
       <c r="A173" t="s" s="2">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B173" s="2"/>
       <c r="C173" t="s" s="2">
@@ -21575,10 +21587,10 @@
         <v>42</v>
       </c>
       <c r="K173" t="s" s="2">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="L173" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M173" s="2"/>
       <c r="N173" s="2"/>
@@ -21629,7 +21641,7 @@
         <v>42</v>
       </c>
       <c r="AE173" t="s" s="2">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="AF173" t="s" s="2">
         <v>50</v>
@@ -21655,7 +21667,7 @@
     </row>
     <row r="174" hidden="true">
       <c r="A174" t="s" s="2">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B174" s="2"/>
       <c r="C174" t="s" s="2">
@@ -21681,10 +21693,10 @@
         <v>371</v>
       </c>
       <c r="K174" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="L174" t="s" s="2">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="M174" s="2"/>
       <c r="N174" s="2"/>
@@ -21735,7 +21747,7 @@
         <v>42</v>
       </c>
       <c r="AE174" t="s" s="2">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="AF174" t="s" s="2">
         <v>40</v>
@@ -21761,7 +21773,7 @@
     </row>
     <row r="175" hidden="true">
       <c r="A175" t="s" s="2">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B175" s="2"/>
       <c r="C175" t="s" s="2">
@@ -21867,7 +21879,7 @@
     </row>
     <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" t="s" s="2">
@@ -21975,7 +21987,7 @@
     </row>
     <row r="177" hidden="true">
       <c r="A177" t="s" s="2">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" t="s" s="2">
@@ -22085,7 +22097,7 @@
     </row>
     <row r="178" hidden="true">
       <c r="A178" t="s" s="2">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B178" s="2"/>
       <c r="C178" t="s" s="2">
@@ -22111,16 +22123,16 @@
         <v>135</v>
       </c>
       <c r="K178" t="s" s="2">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="L178" t="s" s="2">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="M178" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="N178" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="O178" t="s" s="2">
         <v>42</v>
@@ -22148,10 +22160,10 @@
         <v>247</v>
       </c>
       <c r="X178" t="s" s="2">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="Y178" t="s" s="2">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="Z178" t="s" s="2">
         <v>42</v>
@@ -22169,7 +22181,7 @@
         <v>42</v>
       </c>
       <c r="AE178" t="s" s="2">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="AF178" t="s" s="2">
         <v>50</v>
@@ -22195,7 +22207,7 @@
     </row>
     <row r="179" hidden="true">
       <c r="A179" t="s" s="2">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B179" s="2"/>
       <c r="C179" t="s" s="2">
@@ -22221,16 +22233,16 @@
         <v>135</v>
       </c>
       <c r="K179" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="L179" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="M179" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="N179" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="O179" t="s" s="2">
         <v>42</v>
@@ -22258,10 +22270,10 @@
         <v>247</v>
       </c>
       <c r="X179" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="Y179" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="Z179" t="s" s="2">
         <v>42</v>
@@ -22279,7 +22291,7 @@
         <v>42</v>
       </c>
       <c r="AE179" t="s" s="2">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="AF179" t="s" s="2">
         <v>40</v>
@@ -22300,12 +22312,12 @@
         <v>42</v>
       </c>
       <c r="AL179" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="180" hidden="true">
       <c r="A180" t="s" s="2">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B180" s="2"/>
       <c r="C180" t="s" s="2">
@@ -22328,17 +22340,17 @@
         <v>42</v>
       </c>
       <c r="J180" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="K180" t="s" s="2">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="L180" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="M180" s="2"/>
       <c r="N180" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="O180" t="s" s="2">
         <v>42</v>
@@ -22387,7 +22399,7 @@
         <v>42</v>
       </c>
       <c r="AE180" t="s" s="2">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="AF180" t="s" s="2">
         <v>40</v>
@@ -22408,12 +22420,12 @@
         <v>42</v>
       </c>
       <c r="AL180" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="181" hidden="true">
       <c r="A181" t="s" s="2">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B181" s="2"/>
       <c r="C181" t="s" s="2">
@@ -22439,14 +22451,14 @@
         <v>414</v>
       </c>
       <c r="K181" t="s" s="2">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="L181" t="s" s="2">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="M181" s="2"/>
       <c r="N181" t="s" s="2">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="O181" t="s" s="2">
         <v>42</v>
@@ -22495,7 +22507,7 @@
         <v>42</v>
       </c>
       <c r="AE181" t="s" s="2">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="AF181" t="s" s="2">
         <v>40</v>
@@ -22521,7 +22533,7 @@
     </row>
     <row r="182" hidden="true">
       <c r="A182" t="s" s="2">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B182" s="2"/>
       <c r="C182" t="s" s="2">
@@ -22547,16 +22559,16 @@
         <v>422</v>
       </c>
       <c r="K182" t="s" s="2">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="L182" t="s" s="2">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="M182" t="s" s="2">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="N182" t="s" s="2">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="O182" t="s" s="2">
         <v>42</v>
@@ -22605,7 +22617,7 @@
         <v>42</v>
       </c>
       <c r="AE182" t="s" s="2">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="AF182" t="s" s="2">
         <v>40</v>
@@ -22631,7 +22643,7 @@
     </row>
     <row r="183" hidden="true">
       <c r="A183" t="s" s="2">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B183" s="2"/>
       <c r="C183" t="s" s="2">
@@ -22657,16 +22669,16 @@
         <v>414</v>
       </c>
       <c r="K183" t="s" s="2">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="L183" t="s" s="2">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="M183" t="s" s="2">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="N183" t="s" s="2">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="O183" t="s" s="2">
         <v>42</v>
@@ -22715,7 +22727,7 @@
         <v>42</v>
       </c>
       <c r="AE183" t="s" s="2">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="AF183" t="s" s="2">
         <v>40</v>
@@ -22736,12 +22748,12 @@
         <v>42</v>
       </c>
       <c r="AL183" t="s" s="2">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="184" hidden="true">
       <c r="A184" t="s" s="2">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B184" s="2"/>
       <c r="C184" t="s" s="2">
@@ -22767,10 +22779,10 @@
         <v>383</v>
       </c>
       <c r="K184" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="L184" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="M184" s="2"/>
       <c r="N184" t="s" s="2">
@@ -22823,7 +22835,7 @@
         <v>42</v>
       </c>
       <c r="AE184" t="s" s="2">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="AF184" t="s" s="2">
         <v>40</v>
@@ -22849,7 +22861,7 @@
     </row>
     <row r="185" hidden="true">
       <c r="A185" t="s" s="2">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B185" s="2"/>
       <c r="C185" t="s" s="2">
@@ -22875,10 +22887,10 @@
         <v>42</v>
       </c>
       <c r="K185" t="s" s="2">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="L185" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M185" s="2"/>
       <c r="N185" s="2"/>
@@ -22929,7 +22941,7 @@
         <v>42</v>
       </c>
       <c r="AE185" t="s" s="2">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="AF185" t="s" s="2">
         <v>50</v>
@@ -22955,7 +22967,7 @@
     </row>
     <row r="186" hidden="true">
       <c r="A186" t="s" s="2">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B186" s="2"/>
       <c r="C186" t="s" s="2">
@@ -22981,14 +22993,14 @@
         <v>42</v>
       </c>
       <c r="K186" t="s" s="2">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="L186" t="s" s="2">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="M186" s="2"/>
       <c r="N186" t="s" s="2">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="O186" t="s" s="2">
         <v>42</v>
@@ -23037,7 +23049,7 @@
         <v>42</v>
       </c>
       <c r="AE186" t="s" s="2">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="AF186" t="s" s="2">
         <v>40</v>
@@ -23063,7 +23075,7 @@
     </row>
     <row r="187" hidden="true">
       <c r="A187" t="s" s="2">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="B187" s="2"/>
       <c r="C187" t="s" s="2">
@@ -23089,16 +23101,16 @@
         <v>371</v>
       </c>
       <c r="K187" t="s" s="2">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="L187" t="s" s="2">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="M187" t="s" s="2">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="N187" t="s" s="2">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="O187" t="s" s="2">
         <v>42</v>
@@ -23147,7 +23159,7 @@
         <v>42</v>
       </c>
       <c r="AE187" t="s" s="2">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="AF187" t="s" s="2">
         <v>40</v>
@@ -23173,7 +23185,7 @@
     </row>
     <row r="188" hidden="true">
       <c r="A188" t="s" s="2">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B188" s="2"/>
       <c r="C188" t="s" s="2">
@@ -23279,7 +23291,7 @@
     </row>
     <row r="189" hidden="true">
       <c r="A189" t="s" s="2">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B189" s="2"/>
       <c r="C189" t="s" s="2">
@@ -23387,7 +23399,7 @@
     </row>
     <row r="190" hidden="true">
       <c r="A190" t="s" s="2">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B190" s="2"/>
       <c r="C190" t="s" s="2">
@@ -23497,7 +23509,7 @@
     </row>
     <row r="191" hidden="true">
       <c r="A191" t="s" s="2">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B191" s="2"/>
       <c r="C191" t="s" s="2">
@@ -23523,16 +23535,16 @@
         <v>135</v>
       </c>
       <c r="K191" t="s" s="2">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="L191" t="s" s="2">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="M191" t="s" s="2">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="N191" t="s" s="2">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="O191" t="s" s="2">
         <v>42</v>
@@ -23560,10 +23572,10 @@
         <v>247</v>
       </c>
       <c r="X191" t="s" s="2">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="Y191" t="s" s="2">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="Z191" t="s" s="2">
         <v>42</v>
@@ -23581,7 +23593,7 @@
         <v>42</v>
       </c>
       <c r="AE191" t="s" s="2">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="AF191" t="s" s="2">
         <v>50</v>
@@ -23607,7 +23619,7 @@
     </row>
     <row r="192" hidden="true">
       <c r="A192" t="s" s="2">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B192" s="2"/>
       <c r="C192" t="s" s="2">
@@ -23633,14 +23645,14 @@
         <v>414</v>
       </c>
       <c r="K192" t="s" s="2">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="L192" t="s" s="2">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="M192" s="2"/>
       <c r="N192" t="s" s="2">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="O192" t="s" s="2">
         <v>42</v>
@@ -23689,7 +23701,7 @@
         <v>42</v>
       </c>
       <c r="AE192" t="s" s="2">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="AF192" t="s" s="2">
         <v>50</v>
@@ -23715,7 +23727,7 @@
     </row>
     <row r="193" hidden="true">
       <c r="A193" t="s" s="2">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B193" s="2"/>
       <c r="C193" t="s" s="2">
@@ -23741,14 +23753,14 @@
         <v>371</v>
       </c>
       <c r="K193" t="s" s="2">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="L193" t="s" s="2">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="M193" s="2"/>
       <c r="N193" t="s" s="2">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="O193" t="s" s="2">
         <v>42</v>
@@ -23797,7 +23809,7 @@
         <v>42</v>
       </c>
       <c r="AE193" t="s" s="2">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="AF193" t="s" s="2">
         <v>40</v>
@@ -23823,7 +23835,7 @@
     </row>
     <row r="194" hidden="true">
       <c r="A194" t="s" s="2">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B194" s="2"/>
       <c r="C194" t="s" s="2">
@@ -23929,7 +23941,7 @@
     </row>
     <row r="195" hidden="true">
       <c r="A195" t="s" s="2">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B195" s="2"/>
       <c r="C195" t="s" s="2">
@@ -24037,7 +24049,7 @@
     </row>
     <row r="196" hidden="true">
       <c r="A196" t="s" s="2">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B196" s="2"/>
       <c r="C196" t="s" s="2">
@@ -24147,7 +24159,7 @@
     </row>
     <row r="197" hidden="true">
       <c r="A197" t="s" s="2">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B197" s="2"/>
       <c r="C197" t="s" s="2">
@@ -24173,14 +24185,14 @@
         <v>135</v>
       </c>
       <c r="K197" t="s" s="2">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="L197" t="s" s="2">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="M197" s="2"/>
       <c r="N197" t="s" s="2">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="O197" t="s" s="2">
         <v>42</v>
@@ -24208,10 +24220,10 @@
         <v>247</v>
       </c>
       <c r="X197" t="s" s="2">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="Y197" t="s" s="2">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="Z197" t="s" s="2">
         <v>42</v>
@@ -24229,7 +24241,7 @@
         <v>42</v>
       </c>
       <c r="AE197" t="s" s="2">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="AF197" t="s" s="2">
         <v>50</v>
@@ -24255,7 +24267,7 @@
     </row>
     <row r="198" hidden="true">
       <c r="A198" t="s" s="2">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B198" s="2"/>
       <c r="C198" t="s" s="2">
@@ -24281,16 +24293,16 @@
         <v>414</v>
       </c>
       <c r="K198" t="s" s="2">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="L198" t="s" s="2">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M198" t="s" s="2">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="N198" t="s" s="2">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="O198" t="s" s="2">
         <v>42</v>
@@ -24339,7 +24351,7 @@
         <v>42</v>
       </c>
       <c r="AE198" t="s" s="2">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="AF198" t="s" s="2">
         <v>40</v>
@@ -24365,7 +24377,7 @@
     </row>
     <row r="199" hidden="true">
       <c r="A199" t="s" s="2">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B199" s="2"/>
       <c r="C199" t="s" s="2">
@@ -24391,14 +24403,14 @@
         <v>135</v>
       </c>
       <c r="K199" t="s" s="2">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="L199" t="s" s="2">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="M199" s="2"/>
       <c r="N199" t="s" s="2">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="O199" t="s" s="2">
         <v>42</v>
@@ -24426,10 +24438,10 @@
         <v>247</v>
       </c>
       <c r="X199" t="s" s="2">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="Y199" t="s" s="2">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="Z199" t="s" s="2">
         <v>42</v>
@@ -24447,7 +24459,7 @@
         <v>42</v>
       </c>
       <c r="AE199" t="s" s="2">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="AF199" t="s" s="2">
         <v>40</v>
@@ -24473,7 +24485,7 @@
     </row>
     <row r="200" hidden="true">
       <c r="A200" t="s" s="2">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B200" s="2"/>
       <c r="C200" t="s" s="2">
@@ -24496,17 +24508,17 @@
         <v>42</v>
       </c>
       <c r="J200" t="s" s="2">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="K200" t="s" s="2">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="L200" t="s" s="2">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="M200" s="2"/>
       <c r="N200" t="s" s="2">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="O200" t="s" s="2">
         <v>42</v>
@@ -24555,7 +24567,7 @@
         <v>42</v>
       </c>
       <c r="AE200" t="s" s="2">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="AF200" t="s" s="2">
         <v>40</v>
@@ -24581,7 +24593,7 @@
     </row>
     <row r="201" hidden="true">
       <c r="A201" t="s" s="2">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B201" s="2"/>
       <c r="C201" t="s" s="2">
@@ -24607,14 +24619,14 @@
         <v>414</v>
       </c>
       <c r="K201" t="s" s="2">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="L201" t="s" s="2">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="M201" s="2"/>
       <c r="N201" t="s" s="2">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="O201" t="s" s="2">
         <v>42</v>
@@ -24663,7 +24675,7 @@
         <v>42</v>
       </c>
       <c r="AE201" t="s" s="2">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="AF201" t="s" s="2">
         <v>50</v>
@@ -24689,7 +24701,7 @@
     </row>
     <row r="202" hidden="true">
       <c r="A202" t="s" s="2">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B202" s="2"/>
       <c r="C202" t="s" s="2">
@@ -24715,16 +24727,16 @@
         <v>108</v>
       </c>
       <c r="K202" t="s" s="2">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="L202" t="s" s="2">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="M202" t="s" s="2">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="N202" t="s" s="2">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="O202" t="s" s="2">
         <v>42</v>
@@ -24773,7 +24785,7 @@
         <v>42</v>
       </c>
       <c r="AE202" t="s" s="2">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="AF202" t="s" s="2">
         <v>40</v>
@@ -24799,7 +24811,7 @@
     </row>
     <row r="203" hidden="true">
       <c r="A203" t="s" s="2">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="B203" s="2"/>
       <c r="C203" t="s" s="2">
@@ -24825,16 +24837,16 @@
         <v>135</v>
       </c>
       <c r="K203" t="s" s="2">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="L203" t="s" s="2">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="M203" t="s" s="2">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="N203" t="s" s="2">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="O203" t="s" s="2">
         <v>42</v>
@@ -24862,10 +24874,10 @@
         <v>247</v>
       </c>
       <c r="X203" t="s" s="2">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="Y203" t="s" s="2">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="Z203" t="s" s="2">
         <v>42</v>
@@ -24883,7 +24895,7 @@
         <v>42</v>
       </c>
       <c r="AE203" t="s" s="2">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="AF203" t="s" s="2">
         <v>40</v>
@@ -24909,7 +24921,7 @@
     </row>
     <row r="204" hidden="true">
       <c r="A204" t="s" s="2">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B204" s="2"/>
       <c r="C204" t="s" s="2">
@@ -24935,16 +24947,16 @@
         <v>135</v>
       </c>
       <c r="K204" t="s" s="2">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="L204" t="s" s="2">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="M204" t="s" s="2">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="N204" t="s" s="2">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="O204" t="s" s="2">
         <v>42</v>
@@ -24972,10 +24984,10 @@
         <v>247</v>
       </c>
       <c r="X204" t="s" s="2">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="Y204" t="s" s="2">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="Z204" t="s" s="2">
         <v>42</v>
@@ -24993,7 +25005,7 @@
         <v>42</v>
       </c>
       <c r="AE204" t="s" s="2">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="AF204" t="s" s="2">
         <v>40</v>
@@ -25019,7 +25031,7 @@
     </row>
     <row r="205" hidden="true">
       <c r="A205" t="s" s="2">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B205" s="2"/>
       <c r="C205" t="s" s="2">
@@ -25042,19 +25054,19 @@
         <v>42</v>
       </c>
       <c r="J205" t="s" s="2">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="K205" t="s" s="2">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="L205" t="s" s="2">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="M205" t="s" s="2">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="N205" t="s" s="2">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="O205" t="s" s="2">
         <v>42</v>
@@ -25103,7 +25115,7 @@
         <v>42</v>
       </c>
       <c r="AE205" t="s" s="2">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="AF205" t="s" s="2">
         <v>40</v>
@@ -25129,14 +25141,14 @@
     </row>
     <row r="206">
       <c r="A206" t="s" s="2">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B206" s="2"/>
       <c r="C206" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D206" t="s" s="2">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="E206" t="s" s="2">
         <v>40</v>
@@ -25157,14 +25169,14 @@
         <v>371</v>
       </c>
       <c r="K206" t="s" s="2">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="L206" t="s" s="2">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="M206" s="2"/>
       <c r="N206" t="s" s="2">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="O206" t="s" s="2">
         <v>42</v>
@@ -25213,7 +25225,7 @@
         <v>42</v>
       </c>
       <c r="AE206" t="s" s="2">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="AF206" t="s" s="2">
         <v>40</v>
@@ -25239,7 +25251,7 @@
     </row>
     <row r="207" hidden="true">
       <c r="A207" t="s" s="2">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B207" s="2"/>
       <c r="C207" t="s" s="2">
@@ -25345,7 +25357,7 @@
     </row>
     <row r="208" hidden="true">
       <c r="A208" t="s" s="2">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B208" s="2"/>
       <c r="C208" t="s" s="2">
@@ -25453,7 +25465,7 @@
     </row>
     <row r="209" hidden="true">
       <c r="A209" t="s" s="2">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B209" s="2"/>
       <c r="C209" t="s" s="2">
@@ -25563,7 +25575,7 @@
     </row>
     <row r="210">
       <c r="A210" t="s" s="2">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B210" s="2"/>
       <c r="C210" t="s" s="2">
@@ -25594,13 +25606,13 @@
         <v>388</v>
       </c>
       <c r="L210" t="s" s="2">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="M210" t="s" s="2">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="N210" t="s" s="2">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="O210" t="s" s="2">
         <v>42</v>
@@ -25649,7 +25661,7 @@
         <v>42</v>
       </c>
       <c r="AE210" t="s" s="2">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="AF210" t="s" s="2">
         <v>40</v>
@@ -25675,7 +25687,7 @@
     </row>
     <row r="211" hidden="true">
       <c r="A211" t="s" s="2">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B211" s="2"/>
       <c r="C211" t="s" s="2">
@@ -25701,14 +25713,14 @@
         <v>69</v>
       </c>
       <c r="K211" t="s" s="2">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="L211" t="s" s="2">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="M211" s="2"/>
       <c r="N211" t="s" s="2">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="O211" t="s" s="2">
         <v>42</v>
@@ -25736,10 +25748,10 @@
         <v>129</v>
       </c>
       <c r="X211" t="s" s="2">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="Y211" t="s" s="2">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="Z211" t="s" s="2">
         <v>42</v>
@@ -25757,7 +25769,7 @@
         <v>42</v>
       </c>
       <c r="AE211" t="s" s="2">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="AF211" t="s" s="2">
         <v>40</v>
@@ -25783,14 +25795,14 @@
     </row>
     <row r="212">
       <c r="A212" t="s" s="2">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B212" s="2"/>
       <c r="C212" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D212" t="s" s="2">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="E212" t="s" s="2">
         <v>50</v>
@@ -25811,14 +25823,14 @@
         <v>52</v>
       </c>
       <c r="K212" t="s" s="2">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="L212" t="s" s="2">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="M212" s="2"/>
       <c r="N212" t="s" s="2">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="O212" t="s" s="2">
         <v>42</v>
@@ -25843,13 +25855,13 @@
         <v>42</v>
       </c>
       <c r="W212" t="s" s="2">
-        <v>42</v>
+        <v>140</v>
       </c>
       <c r="X212" t="s" s="2">
-        <v>42</v>
+        <v>782</v>
       </c>
       <c r="Y212" t="s" s="2">
-        <v>42</v>
+        <v>783</v>
       </c>
       <c r="Z212" t="s" s="2">
         <v>42</v>
@@ -25867,7 +25879,7 @@
         <v>42</v>
       </c>
       <c r="AE212" t="s" s="2">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="AF212" t="s" s="2">
         <v>50</v>
@@ -25893,7 +25905,7 @@
     </row>
     <row r="213" hidden="true">
       <c r="A213" t="s" s="2">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="B213" s="2"/>
       <c r="C213" t="s" s="2">
@@ -25919,16 +25931,16 @@
         <v>135</v>
       </c>
       <c r="K213" t="s" s="2">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="L213" t="s" s="2">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c r="M213" t="s" s="2">
-        <v>784</v>
+        <v>787</v>
       </c>
       <c r="N213" t="s" s="2">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="O213" t="s" s="2">
         <v>42</v>
@@ -25977,7 +25989,7 @@
         <v>42</v>
       </c>
       <c r="AE213" t="s" s="2">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="AF213" t="s" s="2">
         <v>40</v>
@@ -26003,7 +26015,7 @@
     </row>
     <row r="214" hidden="true">
       <c r="A214" t="s" s="2">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="B214" s="2"/>
       <c r="C214" t="s" s="2">
@@ -26026,19 +26038,19 @@
         <v>42</v>
       </c>
       <c r="J214" t="s" s="2">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="K214" t="s" s="2">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="L214" t="s" s="2">
-        <v>789</v>
+        <v>792</v>
       </c>
       <c r="M214" t="s" s="2">
-        <v>790</v>
+        <v>793</v>
       </c>
       <c r="N214" t="s" s="2">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c r="O214" t="s" s="2">
         <v>42</v>
@@ -26087,7 +26099,7 @@
         <v>42</v>
       </c>
       <c r="AE214" t="s" s="2">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="AF214" t="s" s="2">
         <v>40</v>
@@ -26113,7 +26125,7 @@
     </row>
     <row r="215">
       <c r="A215" t="s" s="2">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="B215" s="2"/>
       <c r="C215" t="s" s="2">
@@ -26139,16 +26151,16 @@
         <v>371</v>
       </c>
       <c r="K215" t="s" s="2">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="L215" t="s" s="2">
-        <v>794</v>
+        <v>797</v>
       </c>
       <c r="M215" t="s" s="2">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="N215" t="s" s="2">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="O215" t="s" s="2">
         <v>42</v>
@@ -26197,7 +26209,7 @@
         <v>42</v>
       </c>
       <c r="AE215" t="s" s="2">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="AF215" t="s" s="2">
         <v>40</v>
@@ -26218,12 +26230,12 @@
         <v>42</v>
       </c>
       <c r="AL215" t="s" s="2">
-        <v>797</v>
+        <v>800</v>
       </c>
     </row>
     <row r="216" hidden="true">
       <c r="A216" t="s" s="2">
-        <v>798</v>
+        <v>801</v>
       </c>
       <c r="B216" s="2"/>
       <c r="C216" t="s" s="2">
@@ -26329,7 +26341,7 @@
     </row>
     <row r="217" hidden="true">
       <c r="A217" t="s" s="2">
-        <v>799</v>
+        <v>802</v>
       </c>
       <c r="B217" s="2"/>
       <c r="C217" t="s" s="2">
@@ -26437,7 +26449,7 @@
     </row>
     <row r="218" hidden="true">
       <c r="A218" t="s" s="2">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="B218" s="2"/>
       <c r="C218" t="s" s="2">
@@ -26547,7 +26559,7 @@
     </row>
     <row r="219">
       <c r="A219" t="s" s="2">
-        <v>801</v>
+        <v>804</v>
       </c>
       <c r="B219" s="2"/>
       <c r="C219" t="s" s="2">
@@ -26573,14 +26585,14 @@
         <v>383</v>
       </c>
       <c r="K219" t="s" s="2">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="L219" t="s" s="2">
-        <v>803</v>
+        <v>806</v>
       </c>
       <c r="M219" s="2"/>
       <c r="N219" t="s" s="2">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c r="O219" t="s" s="2">
         <v>42</v>
@@ -26629,7 +26641,7 @@
         <v>42</v>
       </c>
       <c r="AE219" t="s" s="2">
-        <v>801</v>
+        <v>804</v>
       </c>
       <c r="AF219" t="s" s="2">
         <v>50</v>
@@ -26655,7 +26667,7 @@
     </row>
     <row r="220">
       <c r="A220" t="s" s="2">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="B220" s="2"/>
       <c r="C220" t="s" s="2">
@@ -26681,16 +26693,16 @@
         <v>229</v>
       </c>
       <c r="K220" t="s" s="2">
-        <v>806</v>
+        <v>809</v>
       </c>
       <c r="L220" t="s" s="2">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c r="M220" t="s" s="2">
-        <v>808</v>
+        <v>811</v>
       </c>
       <c r="N220" t="s" s="2">
-        <v>809</v>
+        <v>812</v>
       </c>
       <c r="O220" t="s" s="2">
         <v>42</v>
@@ -26739,7 +26751,7 @@
         <v>42</v>
       </c>
       <c r="AE220" t="s" s="2">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="AF220" t="s" s="2">
         <v>50</v>
@@ -26765,14 +26777,14 @@
     </row>
     <row r="221">
       <c r="A221" t="s" s="2">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="B221" s="2"/>
       <c r="C221" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D221" t="s" s="2">
-        <v>811</v>
+        <v>814</v>
       </c>
       <c r="E221" t="s" s="2">
         <v>50</v>
@@ -26790,17 +26802,17 @@
         <v>42</v>
       </c>
       <c r="J221" t="s" s="2">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="K221" t="s" s="2">
-        <v>811</v>
+        <v>814</v>
       </c>
       <c r="L221" t="s" s="2">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="M221" s="2"/>
       <c r="N221" t="s" s="2">
-        <v>814</v>
+        <v>817</v>
       </c>
       <c r="O221" t="s" s="2">
         <v>42</v>
@@ -26849,7 +26861,7 @@
         <v>42</v>
       </c>
       <c r="AE221" t="s" s="2">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="AF221" t="s" s="2">
         <v>50</v>
@@ -26875,7 +26887,7 @@
     </row>
     <row r="222" hidden="true">
       <c r="A222" t="s" s="2">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c r="B222" s="2"/>
       <c r="C222" t="s" s="2">
@@ -26901,14 +26913,14 @@
         <v>52</v>
       </c>
       <c r="K222" t="s" s="2">
-        <v>816</v>
+        <v>819</v>
       </c>
       <c r="L222" t="s" s="2">
-        <v>817</v>
+        <v>820</v>
       </c>
       <c r="M222" s="2"/>
       <c r="N222" t="s" s="2">
-        <v>818</v>
+        <v>821</v>
       </c>
       <c r="O222" t="s" s="2">
         <v>42</v>
@@ -26957,7 +26969,7 @@
         <v>42</v>
       </c>
       <c r="AE222" t="s" s="2">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c r="AF222" t="s" s="2">
         <v>40</v>
@@ -26983,7 +26995,7 @@
     </row>
     <row r="223" hidden="true">
       <c r="A223" t="s" s="2">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="B223" s="2"/>
       <c r="C223" t="s" s="2">
@@ -27006,19 +27018,19 @@
         <v>42</v>
       </c>
       <c r="J223" t="s" s="2">
-        <v>820</v>
+        <v>823</v>
       </c>
       <c r="K223" t="s" s="2">
-        <v>821</v>
+        <v>824</v>
       </c>
       <c r="L223" t="s" s="2">
-        <v>822</v>
+        <v>825</v>
       </c>
       <c r="M223" t="s" s="2">
-        <v>823</v>
+        <v>826</v>
       </c>
       <c r="N223" t="s" s="2">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="O223" t="s" s="2">
         <v>42</v>
@@ -27067,7 +27079,7 @@
         <v>42</v>
       </c>
       <c r="AE223" t="s" s="2">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="AF223" t="s" s="2">
         <v>40</v>
@@ -27093,14 +27105,14 @@
     </row>
     <row r="224">
       <c r="A224" t="s" s="2">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="B224" s="2"/>
       <c r="C224" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D224" t="s" s="2">
-        <v>826</v>
+        <v>829</v>
       </c>
       <c r="E224" t="s" s="2">
         <v>40</v>
@@ -27121,16 +27133,16 @@
         <v>371</v>
       </c>
       <c r="K224" t="s" s="2">
-        <v>826</v>
+        <v>829</v>
       </c>
       <c r="L224" t="s" s="2">
-        <v>827</v>
+        <v>830</v>
       </c>
       <c r="M224" t="s" s="2">
-        <v>828</v>
+        <v>831</v>
       </c>
       <c r="N224" t="s" s="2">
-        <v>829</v>
+        <v>832</v>
       </c>
       <c r="O224" t="s" s="2">
         <v>42</v>
@@ -27179,7 +27191,7 @@
         <v>42</v>
       </c>
       <c r="AE224" t="s" s="2">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="AF224" t="s" s="2">
         <v>40</v>
@@ -27205,7 +27217,7 @@
     </row>
     <row r="225" hidden="true">
       <c r="A225" t="s" s="2">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c r="B225" s="2"/>
       <c r="C225" t="s" s="2">
@@ -27311,7 +27323,7 @@
     </row>
     <row r="226" hidden="true">
       <c r="A226" t="s" s="2">
-        <v>831</v>
+        <v>834</v>
       </c>
       <c r="B226" s="2"/>
       <c r="C226" t="s" s="2">
@@ -27419,7 +27431,7 @@
     </row>
     <row r="227" hidden="true">
       <c r="A227" t="s" s="2">
-        <v>832</v>
+        <v>835</v>
       </c>
       <c r="B227" s="2"/>
       <c r="C227" t="s" s="2">
@@ -27529,7 +27541,7 @@
     </row>
     <row r="228" hidden="true">
       <c r="A228" t="s" s="2">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c r="B228" s="2"/>
       <c r="C228" t="s" s="2">
@@ -27555,14 +27567,14 @@
         <v>383</v>
       </c>
       <c r="K228" t="s" s="2">
-        <v>834</v>
+        <v>837</v>
       </c>
       <c r="L228" t="s" s="2">
-        <v>835</v>
+        <v>838</v>
       </c>
       <c r="M228" s="2"/>
       <c r="N228" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="O228" t="s" s="2">
         <v>42</v>
@@ -27611,7 +27623,7 @@
         <v>42</v>
       </c>
       <c r="AE228" t="s" s="2">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c r="AF228" t="s" s="2">
         <v>40</v>
@@ -27637,7 +27649,7 @@
     </row>
     <row r="229" hidden="true">
       <c r="A229" t="s" s="2">
-        <v>836</v>
+        <v>839</v>
       </c>
       <c r="B229" s="2"/>
       <c r="C229" t="s" s="2">
@@ -27663,14 +27675,14 @@
         <v>383</v>
       </c>
       <c r="K229" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="L229" t="s" s="2">
-        <v>837</v>
+        <v>840</v>
       </c>
       <c r="M229" s="2"/>
       <c r="N229" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="O229" t="s" s="2">
         <v>42</v>
@@ -27719,7 +27731,7 @@
         <v>42</v>
       </c>
       <c r="AE229" t="s" s="2">
-        <v>836</v>
+        <v>839</v>
       </c>
       <c r="AF229" t="s" s="2">
         <v>40</v>
@@ -27745,7 +27757,7 @@
     </row>
     <row r="230" hidden="true">
       <c r="A230" t="s" s="2">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="B230" s="2"/>
       <c r="C230" t="s" s="2">
@@ -27771,14 +27783,14 @@
         <v>383</v>
       </c>
       <c r="K230" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="L230" t="s" s="2">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c r="M230" s="2"/>
       <c r="N230" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="O230" t="s" s="2">
         <v>42</v>
@@ -27827,7 +27839,7 @@
         <v>42</v>
       </c>
       <c r="AE230" t="s" s="2">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="AF230" t="s" s="2">
         <v>40</v>
@@ -27853,14 +27865,14 @@
     </row>
     <row r="231">
       <c r="A231" t="s" s="2">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="B231" s="2"/>
       <c r="C231" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D231" t="s" s="2">
-        <v>841</v>
+        <v>844</v>
       </c>
       <c r="E231" t="s" s="2">
         <v>50</v>
@@ -27881,14 +27893,14 @@
         <v>135</v>
       </c>
       <c r="K231" t="s" s="2">
-        <v>841</v>
+        <v>844</v>
       </c>
       <c r="L231" t="s" s="2">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c r="M231" s="2"/>
       <c r="N231" t="s" s="2">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c r="O231" t="s" s="2">
         <v>42</v>
@@ -27913,13 +27925,13 @@
         <v>42</v>
       </c>
       <c r="W231" t="s" s="2">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="X231" t="s" s="2">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c r="Y231" t="s" s="2">
-        <v>42</v>
+        <v>848</v>
       </c>
       <c r="Z231" t="s" s="2">
         <v>42</v>
@@ -27937,7 +27949,7 @@
         <v>42</v>
       </c>
       <c r="AE231" t="s" s="2">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="AF231" t="s" s="2">
         <v>50</v>
@@ -27963,7 +27975,7 @@
     </row>
     <row r="232" hidden="true">
       <c r="A232" t="s" s="2">
-        <v>845</v>
+        <v>849</v>
       </c>
       <c r="B232" s="2"/>
       <c r="C232" t="s" s="2">
@@ -28069,7 +28081,7 @@
     </row>
     <row r="233" hidden="true">
       <c r="A233" t="s" s="2">
-        <v>846</v>
+        <v>850</v>
       </c>
       <c r="B233" s="2"/>
       <c r="C233" t="s" s="2">
@@ -28177,7 +28189,7 @@
     </row>
     <row r="234">
       <c r="A234" t="s" s="2">
-        <v>847</v>
+        <v>851</v>
       </c>
       <c r="B234" s="2"/>
       <c r="C234" t="s" s="2">
@@ -28287,7 +28299,7 @@
     </row>
     <row r="235" hidden="true">
       <c r="A235" t="s" s="2">
-        <v>848</v>
+        <v>852</v>
       </c>
       <c r="B235" s="2"/>
       <c r="C235" t="s" s="2">
@@ -28393,7 +28405,7 @@
     </row>
     <row r="236" hidden="true">
       <c r="A236" t="s" s="2">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="B236" s="2"/>
       <c r="C236" t="s" s="2">
@@ -28501,7 +28513,7 @@
     </row>
     <row r="237">
       <c r="A237" t="s" s="2">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c r="B237" s="2"/>
       <c r="C237" t="s" s="2">
@@ -28611,7 +28623,7 @@
     </row>
     <row r="238" hidden="true">
       <c r="A238" t="s" s="2">
-        <v>851</v>
+        <v>855</v>
       </c>
       <c r="B238" s="2"/>
       <c r="C238" t="s" s="2">
@@ -28719,14 +28731,14 @@
     </row>
     <row r="239">
       <c r="A239" t="s" s="2">
-        <v>852</v>
+        <v>856</v>
       </c>
       <c r="B239" s="2"/>
       <c r="C239" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D239" t="s" s="2">
-        <v>853</v>
+        <v>857</v>
       </c>
       <c r="E239" t="s" s="2">
         <v>50</v>
@@ -28747,7 +28759,7 @@
         <v>69</v>
       </c>
       <c r="K239" t="s" s="2">
-        <v>853</v>
+        <v>857</v>
       </c>
       <c r="L239" t="s" s="2">
         <v>218</v>
@@ -28829,7 +28841,7 @@
     </row>
     <row r="240">
       <c r="A240" t="s" s="2">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="B240" s="2"/>
       <c r="C240" t="s" s="2">
@@ -28937,7 +28949,7 @@
     </row>
     <row r="241" hidden="true">
       <c r="A241" t="s" s="2">
-        <v>855</v>
+        <v>859</v>
       </c>
       <c r="B241" s="2"/>
       <c r="C241" t="s" s="2">
@@ -29047,14 +29059,14 @@
     </row>
     <row r="242">
       <c r="A242" t="s" s="2">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c r="B242" s="2"/>
       <c r="C242" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D242" t="s" s="2">
-        <v>857</v>
+        <v>861</v>
       </c>
       <c r="E242" t="s" s="2">
         <v>40</v>
@@ -29075,10 +29087,10 @@
         <v>52</v>
       </c>
       <c r="K242" t="s" s="2">
-        <v>857</v>
+        <v>861</v>
       </c>
       <c r="L242" t="s" s="2">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="M242" t="s" s="2">
         <v>239</v>

</xml_diff>